<commit_message>
Update the tables download files
</commit_message>
<xml_diff>
--- a/input/images/tables/codesystem-ref-all-list.xlsx
+++ b/input/images/tables/codesystem-ref-all-list.xlsx
@@ -1523,42 +1523,42 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>http://hl7.org/fhir/fhir-types</t>
+          <t>http://hl7.org/fhir/fm-status</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>5.0.0</t>
+          <t>4.0.1</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.4.1802</t>
+          <t>2.16.840.1.113883.4.642.4.593</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>FHIRTypes</t>
+          <t>FinancialResourceStatusCodes</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>All FHIR Types</t>
+          <t>Financial Resource Status Codes</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>One of the types defined as part of this version of FHIR.</t>
+          <t>This value set includes Status codes.</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>ValueSet/resource-types</t>
+          <t>ValueSet/fm-status</t>
         </is>
       </c>
       <c r="I26" t="inlineStr"/>
@@ -1567,7 +1567,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>http://hl7.org/fhir/fm-status</t>
+          <t>http://hl7.org/fhir/goal-status</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1582,27 +1582,27 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.4.593</t>
+          <t>2.16.840.1.113883.4.642.4.272</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>FinancialResourceStatusCodes</t>
+          <t>GoalLifecycleStatus</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Financial Resource Status Codes</t>
+          <t>GoalLifecycleStatus</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>This value set includes Status codes.</t>
+          <t>Codes that reflect the current state of a goal and whether the goal is still being targeted.</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>ValueSet/fm-status</t>
+          <t>ValueSet/goal-status</t>
         </is>
       </c>
       <c r="I27" t="inlineStr"/>
@@ -1611,7 +1611,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>http://hl7.org/fhir/goal-status</t>
+          <t>http://hl7.org/fhir/identifier-use</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1621,32 +1621,32 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>draft</t>
+          <t>active</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.4.272</t>
+          <t>2.16.840.1.113883.4.642.4.58</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>GoalLifecycleStatus</t>
+          <t>IdentifierUse</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>GoalLifecycleStatus</t>
+          <t>IdentifierUse</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Codes that reflect the current state of a goal and whether the goal is still being targeted.</t>
+          <t>Identifies the purpose for this identifier, if known .</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>ValueSet/goal-status</t>
+          <t>ValueSet/identifier-use</t>
         </is>
       </c>
       <c r="I28" t="inlineStr"/>
@@ -1655,7 +1655,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>http://hl7.org/fhir/identifier-use</t>
+          <t>http://hl7.org/fhir/link-type</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1670,27 +1670,27 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.4.58</t>
+          <t>2.16.840.1.113883.4.642.4.424</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>IdentifierUse</t>
+          <t>LinkType</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>IdentifierUse</t>
+          <t>LinkType</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Identifies the purpose for this identifier, if known .</t>
+          <t>The type of link between this patient resource and another patient resource.</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>ValueSet/identifier-use</t>
+          <t>ValueSet/link-type</t>
         </is>
       </c>
       <c r="I29" t="inlineStr"/>
@@ -1699,7 +1699,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>http://hl7.org/fhir/link-type</t>
+          <t>http://hl7.org/fhir/location-mode</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1709,32 +1709,32 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.4.424</t>
+          <t>2.16.840.1.113883.4.642.4.331</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>LinkType</t>
+          <t>LocationMode</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>LinkType</t>
+          <t>LocationMode</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>The type of link between this patient resource and another patient resource.</t>
+          <t>Indicates whether a resource instance represents a specific location or a class of locations.</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>ValueSet/link-type</t>
+          <t>ValueSet/location-mode</t>
         </is>
       </c>
       <c r="I30" t="inlineStr"/>
@@ -1743,7 +1743,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>http://hl7.org/fhir/location-mode</t>
+          <t>http://hl7.org/fhir/location-status</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1758,27 +1758,27 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.4.331</t>
+          <t>2.16.840.1.113883.4.642.4.333</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>LocationMode</t>
+          <t>LocationStatus</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>LocationMode</t>
+          <t>LocationStatus</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Indicates whether a resource instance represents a specific location or a class of locations.</t>
+          <t>Indicates whether the location is still in use.</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>ValueSet/location-mode</t>
+          <t>ValueSet/location-status</t>
         </is>
       </c>
       <c r="I31" t="inlineStr"/>
@@ -1787,7 +1787,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>http://hl7.org/fhir/location-status</t>
+          <t>http://hl7.org/fhir/name-use</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1797,32 +1797,32 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>draft</t>
+          <t>active</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.4.333</t>
+          <t>2.16.840.1.113883.4.642.4.66</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>LocationStatus</t>
+          <t>NameUse</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>LocationStatus</t>
+          <t>NameUse</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Indicates whether the location is still in use.</t>
+          <t>The use of a human name.</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>ValueSet/location-status</t>
+          <t>ValueSet/name-use</t>
         </is>
       </c>
       <c r="I32" t="inlineStr"/>
@@ -1831,7 +1831,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>http://hl7.org/fhir/name-use</t>
+          <t>http://hl7.org/fhir/narrative-status</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1841,32 +1841,32 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.4.66</t>
+          <t>2.16.840.1.113883.4.642.4.56</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>NameUse</t>
+          <t>NarrativeStatus</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>NameUse</t>
+          <t>NarrativeStatus</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>The use of a human name.</t>
+          <t>The status of a resource narrative.</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>ValueSet/name-use</t>
+          <t>ValueSet/us-core-narrative-status</t>
         </is>
       </c>
       <c r="I33" t="inlineStr"/>
@@ -1875,7 +1875,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>http://hl7.org/fhir/narrative-status</t>
+          <t>http://hl7.org/fhir/observation-status</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1885,32 +1885,32 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>draft</t>
+          <t>active</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.4.56</t>
+          <t>2.16.840.1.113883.4.642.4.401</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>NarrativeStatus</t>
+          <t>ObservationStatus</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>NarrativeStatus</t>
+          <t>ObservationStatus</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>The status of a resource narrative.</t>
+          <t>Codes providing the status of an observation.</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>ValueSet/us-core-narrative-status</t>
+          <t>ValueSet/us-core-observation-smoking-status-status,ValueSet/observation-status</t>
         </is>
       </c>
       <c r="I34" t="inlineStr"/>
@@ -1919,7 +1919,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>http://hl7.org/fhir/observation-status</t>
+          <t>http://hl7.org/fhir/provenance-entity-role</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1929,32 +1929,32 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.4.401</t>
+          <t>2.16.840.1.113883.4.642.4.437</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>ObservationStatus</t>
+          <t>ProvenanceEntityRole</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>ObservationStatus</t>
+          <t>ProvenanceEntityRole</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Codes providing the status of an observation.</t>
+          <t>How an entity was used in an activity.</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>ValueSet/us-core-observation-smoking-status-status,ValueSet/observation-status</t>
+          <t>ValueSet/provenance-entity-role</t>
         </is>
       </c>
       <c r="I35" t="inlineStr"/>
@@ -1963,7 +1963,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>http://hl7.org/fhir/provenance-entity-role</t>
+          <t>http://hl7.org/fhir/quantity-comparator</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1973,32 +1973,32 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>draft</t>
+          <t>active</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.4.437</t>
+          <t>2.16.840.1.113883.4.642.4.60</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>ProvenanceEntityRole</t>
+          <t>QuantityComparator</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>ProvenanceEntityRole</t>
+          <t>QuantityComparator</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>How an entity was used in an activity.</t>
+          <t>How the Quantity should be understood and represented.</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>ValueSet/provenance-entity-role</t>
+          <t>ValueSet/quantity-comparator</t>
         </is>
       </c>
       <c r="I36" t="inlineStr"/>
@@ -2007,7 +2007,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>http://hl7.org/fhir/quantity-comparator</t>
+          <t>http://hl7.org/fhir/questionnaire-answers-status</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -2017,32 +2017,32 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.4.60</t>
+          <t>2.16.840.1.113883.4.642.4.448</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>QuantityComparator</t>
+          <t>QuestionnaireResponseStatus</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>QuantityComparator</t>
+          <t>QuestionnaireResponseStatus</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>How the Quantity should be understood and represented.</t>
+          <t>Lifecycle status of the questionnaire response.</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>ValueSet/quantity-comparator</t>
+          <t>ValueSet/questionnaire-answers-status</t>
         </is>
       </c>
       <c r="I37" t="inlineStr"/>
@@ -2051,7 +2051,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>http://hl7.org/fhir/questionnaire-answers-status</t>
+          <t>http://hl7.org/fhir/reaction-event-severity</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -2066,27 +2066,27 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.4.448</t>
+          <t>2.16.840.1.113883.4.642.4.136</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>QuestionnaireResponseStatus</t>
+          <t>AllergyIntoleranceSeverity</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>QuestionnaireResponseStatus</t>
+          <t>AllergyIntoleranceSeverity</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Lifecycle status of the questionnaire response.</t>
+          <t>Clinical assessment of the severity of a reaction event as a whole, potentially considering multiple different manifestations.</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>ValueSet/questionnaire-answers-status</t>
+          <t>ValueSet/reaction-event-severity</t>
         </is>
       </c>
       <c r="I38" t="inlineStr"/>
@@ -2095,7 +2095,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>http://hl7.org/fhir/reaction-event-severity</t>
+          <t>http://hl7.org/fhir/request-intent</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -2110,27 +2110,27 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.4.136</t>
+          <t>2.16.840.1.113883.4.642.4.114</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>AllergyIntoleranceSeverity</t>
+          <t>RequestIntent</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>AllergyIntoleranceSeverity</t>
+          <t>RequestIntent</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Clinical assessment of the severity of a reaction event as a whole, potentially considering multiple different manifestations.</t>
+          <t>Codes indicating the degree of authority/intentionality associated with a request.</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>ValueSet/reaction-event-severity</t>
+          <t>ValueSet/request-intent,ValueSet/care-plan-intent</t>
         </is>
       </c>
       <c r="I39" t="inlineStr"/>
@@ -2139,7 +2139,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>http://hl7.org/fhir/request-intent</t>
+          <t>http://hl7.org/fhir/request-priority</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -2154,27 +2154,27 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.4.114</t>
+          <t>2.16.840.1.113883.4.642.4.116</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>RequestIntent</t>
+          <t>RequestPriority</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>RequestIntent</t>
+          <t>RequestPriority</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Codes indicating the degree of authority/intentionality associated with a request.</t>
+          <t>Identifies the level of importance to be assigned to actioning the request.</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>ValueSet/request-intent,ValueSet/care-plan-intent</t>
+          <t>ValueSet/request-priority</t>
         </is>
       </c>
       <c r="I40" t="inlineStr"/>
@@ -2183,7 +2183,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>http://hl7.org/fhir/request-priority</t>
+          <t>http://hl7.org/fhir/request-status</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -2198,27 +2198,27 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.4.116</t>
+          <t>2.16.840.1.113883.4.642.4.112</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>RequestPriority</t>
+          <t>RequestStatus</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>RequestPriority</t>
+          <t>RequestStatus</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Identifies the level of importance to be assigned to actioning the request.</t>
+          <t>Codes identifying the lifecycle stage of a request.</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>ValueSet/request-priority</t>
+          <t>ValueSet/request-status</t>
         </is>
       </c>
       <c r="I41" t="inlineStr"/>
@@ -2227,7 +2227,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>http://hl7.org/fhir/request-status</t>
+          <t>http://hl7.org/fhir/resource-types</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -2237,32 +2237,28 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>draft</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>2.16.840.1.113883.4.642.4.112</t>
-        </is>
-      </c>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr">
         <is>
-          <t>RequestStatus</t>
+          <t>ResourceType</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>RequestStatus</t>
+          <t>ResourceType</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Codes identifying the lifecycle stage of a request.</t>
+          <t>One of the resource types defined as part of this version of FHIR.</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>ValueSet/request-status</t>
+          <t>ValueSet/resource-types,ValueSet/care-plan-activity-kind</t>
         </is>
       </c>
       <c r="I42" t="inlineStr"/>
@@ -2271,12 +2267,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>http://hl7.org/fhir/resource-types</t>
+          <t>http://hl7.org/fhir/sid/cvx</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>4.0.1</t>
+          <t>4.0.0</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2284,25 +2280,29 @@
           <t>active</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr"/>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>2.16.840.1.113883.12.292</t>
+        </is>
+      </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>ResourceType</t>
+          <t>CVX</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>ResourceType</t>
+          <t>Vaccine Administered Code Set (CVX)</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>One of the resource types defined as part of this version of FHIR.</t>
+          <t>The CDC's National Center of Immunization and Respiratory Diseases (NCIRD - see [https://www.cdc.gov/ncird/](https://www.cdc.gov/ncird/)) developed and maintains the CVX (vaccine administered) code set. It includes both active and inactive vaccines available in the US. CVX codes for inactive vaccines allow transmission of historical immunization records. When a MVX (manufacturer) code is paired with a CVX (vaccine administered) code, the specific trade named vaccine may be indicated. These codes should be used for immunization messages using either HL7 Version 2.3.1 or HL7 Version 2.5.1. CVX is the underlying Master Code System for V2 table 0292 (Vaccines Administered). The machine readable name for CVX in PHIN VADS is PH_VaccinesAdministeredCVX_CDC_NIP. The version of the CVX code set for certification can be found on the archive page:[https://www2a.cdc.gov/vaccines/iis/iisstandards/mu3versioned_codes.asp](https://www2a.cdc.gov/vaccines/iis/iisstandards/mu3versioned_codes.asp)     The Status column indicates if the vaccine is currently available in the United States.    *  Active: A currently available administrable vaccine     *  Inactive: An administrable vaccine formulation that is no longer available for patient administration, but can be found in historical patient records OR A historical record of a vaccine administered where the exact formulation is unknown     *  Pending: A vaccine that is expected to become active in the future     *  Non-US: A vaccine that available outside the US only     *  Never Active: A vaccine that was never available and is not in the pipeline of new vaccines     The Last Updated column indicates the last time this particular vaccine code was updated in this table.    Questions regarding this table should be directed to the IIS Technical Assistance Team via iisinfo@cdc.gov (or use mailing address via [https://www2a.cdc.gov/vaccines/iis/iisstandards/vaccines.asp?rpt=cvx#addr](https://www2a.cdc.gov/vaccines/iis/iisstandards/vaccines.asp?rpt=cvx#addr))     HL7 Implementers should note that 'Status' IS NOT CONCEPT STATUS as all codes are ACTIVE in this code system.    The current code system is available via [https://www2a.cdc.gov/vaccines/iis/iisstandards/vaccines.asp?rpt=cvx](https://www2a.cdc.gov/vaccines/iis/iisstandards/vaccines.asp?rpt=cvx)</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>ValueSet/care-plan-activity-kind</t>
+          <t>ValueSet/2.16.840.1.113762.1.4.1010.6</t>
         </is>
       </c>
       <c r="I43" t="inlineStr"/>
@@ -2311,12 +2311,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>http://hl7.org/fhir/sid/cvx</t>
+          <t>http://hl7.org/fhir/sid/icd-10-cm</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>4.0.0</t>
+          <t>2.0.1</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -2326,88 +2326,88 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.12.292</t>
+          <t>2.16.840.1.113883.6.90</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>CVX</t>
+          <t>Icd10CM</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Vaccine Administered Code Set (CVX)</t>
+          <t>International Classification of Diseases</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>The CDC's National Center of Immunization and Respiratory Diseases (NCIRD - see [https://www.cdc.gov/ncird/](https://www.cdc.gov/ncird/)) developed and maintains the CVX (vaccine administered) code set. It includes both active and inactive vaccines available in the US. CVX codes for inactive vaccines allow transmission of historical immunization records. When a MVX (manufacturer) code is paired with a CVX (vaccine administered) code, the specific trade named vaccine may be indicated. These codes should be used for immunization messages using either HL7 Version 2.3.1 or HL7 Version 2.5.1. CVX is the underlying Master Code System for V2 table 0292 (Vaccines Administered). The machine readable name for CVX in PHIN VADS is PH_VaccinesAdministeredCVX_CDC_NIP. The version of the CVX code set for certification can be found on the archive page:[https://www2a.cdc.gov/vaccines/iis/iisstandards/mu3versioned_codes.asp](https://www2a.cdc.gov/vaccines/iis/iisstandards/mu3versioned_codes.asp)     The Status column indicates if the vaccine is currently available in the United States.    *  Active: A currently available administrable vaccine     *  Inactive: An administrable vaccine formulation that is no longer available for patient administration, but can be found in historical patient records OR A historical record of a vaccine administered where the exact formulation is unknown     *  Pending: A vaccine that is expected to become active in the future     *  Non-US: A vaccine that available outside the US only     *  Never Active: A vaccine that was never available and is not in the pipeline of new vaccines     The Last Updated column indicates the last time this particular vaccine code was updated in this table.    Questions regarding this table should be directed to the IIS Technical Assistance Team via iisinfo@cdc.gov (or use mailing address via [https://www2a.cdc.gov/vaccines/iis/iisstandards/vaccines.asp?rpt=cvx#addr](https://www2a.cdc.gov/vaccines/iis/iisstandards/vaccines.asp?rpt=cvx#addr))     HL7 Implementers should note that 'Status' IS NOT CONCEPT STATUS as all codes are ACTIVE in this code system.    The current code system is available via [https://www2a.cdc.gov/vaccines/iis/iisstandards/vaccines.asp?rpt=cvx](https://www2a.cdc.gov/vaccines/iis/iisstandards/vaccines.asp?rpt=cvx)</t>
+          <t xml:space="preserve"> 10th Revision</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>ValueSet/2.16.840.1.113762.1.4.1010.6</t>
-        </is>
-      </c>
-      <c r="I44" t="inlineStr"/>
-      <c r="J44" t="inlineStr"/>
+          <t xml:space="preserve"> Clinical Modification (ICD-10-CM)</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>The International Classification of Diseases, 10th Revision, Clinical Modification (ICD-10-CM), describes the classification of morbidity and mortality information for statistical purposes and for the indexing of healthcare records by diseases. The ICD-10-CM codes can be used as the value of the Act.cd attribute.</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>ValueSet/us-core-condition-code</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>http://hl7.org/fhir/sid/icd-10-cm</t>
+          <t>http://hl7.org/fhir/specimen-status</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>2.0.1</t>
+          <t>4.0.1</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.6.90</t>
+          <t>2.16.840.1.113883.4.642.4.472</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Icd10CM</t>
+          <t>SpecimenStatus</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>International Classification of Diseases</t>
+          <t>SpecimenStatus</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 10th Revision</t>
+          <t>Codes providing the status/availability of a specimen.</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Clinical Modification (ICD-10-CM)</t>
-        </is>
-      </c>
-      <c r="I45" t="inlineStr">
-        <is>
-          <t>The International Classification of Diseases, 10th Revision, Clinical Modification (ICD-10-CM), describes the classification of morbidity and mortality information for statistical purposes and for the indexing of healthcare records by diseases. The ICD-10-CM codes can be used as the value of the Act.cd attribute.</t>
-        </is>
-      </c>
-      <c r="J45" t="inlineStr">
-        <is>
-          <t>ValueSet/us-core-condition-code</t>
-        </is>
-      </c>
+          <t>ValueSet/specimen-status</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr"/>
+      <c r="J45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>http://hl7.org/fhir/specimen-status</t>
+          <t>http://hl7.org/fhir/udi-entry-type</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -2422,27 +2422,27 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.4.472</t>
+          <t>2.16.840.1.113883.4.642.4.212</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>SpecimenStatus</t>
+          <t>UDIEntryType</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>SpecimenStatus</t>
+          <t>UDIEntryType</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Codes providing the status/availability of a specimen.</t>
+          <t>Codes to identify how UDI data was entered.</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>ValueSet/specimen-status</t>
+          <t>ValueSet/udi-entry-type</t>
         </is>
       </c>
       <c r="I46" t="inlineStr"/>
@@ -2451,42 +2451,42 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>http://hl7.org/fhir/udi-entry-type</t>
+          <t>http://hl7.org/fhir/us/core/CodeSystem/condition-category</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>4.0.1</t>
+          <t>7.0.0</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>draft</t>
+          <t>active</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.4.212</t>
+          <t>2.16.840.1.113883.4.642.40.2.16.2</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>UDIEntryType</t>
+          <t>USCoreConditionCategoryExtensionCodes</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>UDIEntryType</t>
+          <t>US Core Condition Category Extension Codes</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Codes to identify how UDI data was entered.</t>
+          <t>Set of codes that are needed for implementation of the US-Core Condition Profile. These codes are used as extensions to the FHIR and US Core value sets.</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>ValueSet/udi-entry-type</t>
+          <t>ValueSet/us-core-problem-or-health-concern</t>
         </is>
       </c>
       <c r="I47" t="inlineStr"/>
@@ -2495,12 +2495,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>http://hl7.org/fhir/us/core/CodeSystem/condition-category</t>
+          <t>http://hl7.org/fhir/us/core/CodeSystem/us-core-category</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>7.0.0-ballot</t>
+          <t>7.0.0</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2508,25 +2508,29 @@
           <t>active</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr"/>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>2.16.840.1.113883.4.642.40.2.16.3</t>
+        </is>
+      </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>USCoreConditionCategoryExtensionCodes</t>
+          <t>USCoreCategory</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>US Core Condition Category Extension Codes</t>
+          <t>US Core Category</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Set of codes that are needed for implementation of the US-Core Condition Profile. These codes are used as extensions to the FHIR and US Core value sets.</t>
+          <t>Category codes used across US Core Profiles and resource types. They are typically used when there is a need for categorization for searching and finding resources or workflow hints.</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>ValueSet/us-core-problem-or-health-concern</t>
+          <t>ValueSet/us-core-screening-assessment-observation-category,ValueSet/us-core-simple-observation-category,ValueSet/us-core-servicerequest-category,ValueSet/us-core-screening-assessment-condition-category</t>
         </is>
       </c>
       <c r="I48" t="inlineStr"/>
@@ -2535,12 +2539,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>http://hl7.org/fhir/us/core/CodeSystem/us-core-category</t>
+          <t>http://hl7.org/fhir/us/core/CodeSystem/us-core-documentreference-category</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>7.0.0-ballot</t>
+          <t>7.0.0</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2548,25 +2552,29 @@
           <t>active</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr"/>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>2.16.840.1.113883.4.642.40.2.16.4</t>
+        </is>
+      </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>USCoreCategory</t>
+          <t>USCoreDocumentReferencesCategoryCodes</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>US Core Category</t>
+          <t>US Core DocumentReferences Category Codes</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Category codes used across US Core Profiles and resource types. They are typically used when there is a need for categorization for searching and finding resources or workflow hints.</t>
+          <t>The US Core DocumentReferences Type Code System is a 'starter set' of categories supported for fetching and storing DocumentReference Resources.</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>ValueSet/us-core-screening-assessment-observation-category,ValueSet/us-core-simple-observation-category,ValueSet/us-core-servicerequest-category,ValueSet/us-core-screening-assessment-condition-category</t>
+          <t>ValueSet/us-core-documentreference-category</t>
         </is>
       </c>
       <c r="I49" t="inlineStr"/>
@@ -2575,12 +2583,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>http://hl7.org/fhir/us/core/CodeSystem/us-core-documentreference-category</t>
+          <t>http://hl7.org/fhir/us/core/CodeSystem/us-core-provenance-participant-type</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>7.0.0-ballot</t>
+          <t>7.0.0</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2588,25 +2596,29 @@
           <t>active</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr"/>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>2.16.840.1.113883.4.642.40.2.16.5</t>
+        </is>
+      </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>USCoreDocumentReferencesCategoryCodes</t>
+          <t>USCoreProvenancePaticipantTypeExtensionCodes</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>US Core DocumentReferences Category Codes</t>
+          <t>US Core Provenance Participant Type Extension Codes</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>The US Core DocumentReferences Type Code System is a 'starter set' of categories supported for fetching and storing DocumentReference Resources.</t>
+          <t>Set of codes that are needed for implementation of the US-Core Provenance Profile. These codes are used as extensions to the FHIR value sets.</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>ValueSet/us-core-documentreference-category</t>
+          <t>ValueSet/us-core-provenance-participant-type</t>
         </is>
       </c>
       <c r="I50" t="inlineStr"/>
@@ -2615,12 +2627,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>http://hl7.org/fhir/us/core/CodeSystem/us-core-provenance-participant-type</t>
+          <t>http://loinc.org</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>7.0.0-ballot</t>
+          <t>3.1.0</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2628,39 +2640,47 @@
           <t>active</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr"/>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>2.16.840.1.113883.6.1</t>
+        </is>
+      </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>USCoreProvenancePaticipantTypeExtensionCodes</t>
+          <t>LOINC</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>US Core Provenance Participant Type Extension Codes</t>
+          <t>Logical Observation Identifiers</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Set of codes that are needed for implementation of the US-Core Provenance Profile. These codes are used as extensions to the FHIR value sets.</t>
+          <t xml:space="preserve"> Names and Codes (LOINC)</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>ValueSet/us-core-provenance-participant-type</t>
-        </is>
-      </c>
-      <c r="I51" t="inlineStr"/>
+          <t>LOINC provides a set of universal names and ID codes for identifying laboratory and clinical test results.1,2 LOINC facilitates the exchange and pooling of results, such as blood hemoglobin, serum potassium, or vital signs, for clinical care, outcomes management, and research. LOINC's universal identifiers (names and codes) can be used in the context of order and observation exchanges between information systems that use syntax standards such as HL73, CEN TC251, ISO TC215, ASTM4, and DICOM. Specifically, the identifier can be used as the coded value for an observation in any other standard that uses the observation/observation value paradigm, whether messages, documents, application programming interface (API), etc. For example, LOINC codes are used widely in the OBX segment Observation Identifier field (OBX-3) of an ORU HL7 (HL7 version 2.x or ASTM 1238-9410) message that may be sent between a Clinical Laboratory Information Management Systems (LIMS) and Electronic Health Record Systems (EHR).5, 6 In this way, LOINC codes provide universal identifiers that allow the exchange of clinical data between heterogeneous computing environments.</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>ValueSet/us-core-diagnosticreport-category,ValueSet/c80-doc-typecodes,ValueSet/us-core-documentreference-type,ValueSet/document-classcodes,ValueSet/2.16.840.1.113883.3.88.12.80.62,ValueSet/simple-observation,ValueSet/us-core-smoking-status-observation-codes,ValueSet/us-core-survey-codes,ValueSet/us-core-clinical-note-type,ValueSet/us-core-goal-description,ValueSet/us-core-laboratory-test-codes,ValueSet/care-team-category,ValueSet/us-core-diagnosticreport-report-and-note-codes,ValueSet/observation-codes,ValueSet/us-core-procedure-code</t>
+        </is>
+      </c>
       <c r="J51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>http://loinc.org</t>
+          <t>http://snomed.info/sct</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>3.1.0</t>
+          <t>null</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2670,45 +2690,41 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.6.1</t>
+          <t>2.16.840.1.113883.6.96</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>LOINC</t>
+          <t>SNOMED_CT</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Logical Observation Identifiers</t>
+          <t>SNOMED CT (all versions)</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Names and Codes (LOINC)</t>
+          <t>SNOMED CT is the most comprehensive and precise clinical health terminology product in the world, owned and distributed around the world by The International Health Terminology Standards Development Organisation (IHTSDO).</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>LOINC provides a set of universal names and ID codes for identifying laboratory and clinical test results.1,2 LOINC facilitates the exchange and pooling of results, such as blood hemoglobin, serum potassium, or vital signs, for clinical care, outcomes management, and research. LOINC's universal identifiers (names and codes) can be used in the context of order and observation exchanges between information systems that use syntax standards such as HL73, CEN TC251, ISO TC215, ASTM4, and DICOM. Specifically, the identifier can be used as the coded value for an observation in any other standard that uses the observation/observation value paradigm, whether messages, documents, application programming interface (API), etc. For example, LOINC codes are used widely in the OBX segment Observation Identifier field (OBX-3) of an ORU HL7 (HL7 version 2.x or ASTM 1238-9410) message that may be sent between a Clinical Laboratory Information Management Systems (LIMS) and Electronic Health Record Systems (EHR).5, 6 In this way, LOINC codes provide universal identifiers that allow the exchange of clinical data between heterogeneous computing environments.</t>
-        </is>
-      </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>ValueSet/us-core-diagnosticreport-category,ValueSet/us-core-vital-signs,ValueSet/c80-doc-typecodes,ValueSet/us-core-documentreference-type,ValueSet/document-classcodes,ValueSet/simple-observation,ValueSet/us-core-smoking-status-observation-codes,ValueSet/us-core-survey-codes,ValueSet/us-core-clinical-note-type,ValueSet/us-core-laboratory-test-codes,ValueSet/us-core-goal-description,ValueSet/us-core-diagnosticreport-report-and-note-codes,ValueSet/care-team-category,ValueSet/observation-codes,ValueSet/us-core-procedure-code</t>
-        </is>
-      </c>
+          <t>ValueSet/servicerequest-category,ValueSet/specimen-container-type,ValueSet/2.16.840.1.113762.1.4.1099.54,ValueSet/procedure-followup,ValueSet/us-core-goal-description,ValueSet/specimen-collection-method,ValueSet/medication-form-codes,ValueSet/body-site,ValueSet/manifestation-or-symptom,ValueSet/procedure-code,ValueSet/goal-start-event,ValueSet/medication-as-needed-reason,ValueSet/c80-facilitycodes,ValueSet/2.16.840.1.113762.1.4.1267.3,ValueSet/immunization-reason,ValueSet/substance-code,ValueSet/simple-observation,ValueSet/care-plan-category,ValueSet/us-core-procedure-code,ValueSet/observation-methods,ValueSet/questionnaire-answers,ValueSet/servicerequest-orderdetail,ValueSet/us-core-encounter-type,ValueSet/clinical-findings,ValueSet/condition-stage,ValueSet/immunization-target-disease,ValueSet/encounter-reason,ValueSet/participant-role,ValueSet/additional-instruction-codes,ValueSet/us-core-observation-value-codes,ValueSet/approach-site-codes,ValueSet/device-action,ValueSet/us-core-condition-code,ValueSet/medication-codes,ValueSet/device-kind,ValueSet/performer-role,ValueSet/us-core-servicerequest-category,ValueSet/c80-practice-codes,ValueSet/referencerange-appliesto,ValueSet/route-codes,ValueSet/procedure-outcome,ValueSet/care-plan-activity-outcome,ValueSet/procedure-category,ValueSet/condition-code,ValueSet/condition-stage-type,ValueSet/immunization-status-reason,ValueSet/procedure-not-performed-reason,ValueSet/administration-method-codes,ValueSet/condition-severity</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr"/>
       <c r="J52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>http://snomed.info/sct</t>
+          <t>http://terminology.hl7.org/CodeSystem/PHOccupationalDataForHealthODH</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>2.0.1</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2718,27 +2734,27 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.6.96</t>
+          <t>2.16.840.1.114222.4.5.327</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>SNOMED_CT</t>
+          <t>PHOccupationalDataForHealthODH</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>SNOMED CT (all versions)</t>
+          <t>Occupational Data for Health (ODH)</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>SNOMED CT is the most comprehensive and precise clinical health terminology product in the world, owned and distributed around the world by The International Health Terminology Standards Development Organisation (IHTSDO).</t>
+          <t>The concepts representing the values supporting Occupational Data for Health, including Job Supervisory Level or Pay Grade (ODH) code system consists of data elements that describe a person's work information, structured to facilitate individual, population, and public health use; not intended to support billing.).</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>ValueSet/servicerequest-category,ValueSet/specimen-container-type,ValueSet/2.16.840.1.113762.1.4.1099.54,ValueSet/2.16.840.1.113883.11.20.9.38,ValueSet/procedure-followup,ValueSet/us-core-goal-description,ValueSet/specimen-collection-method,ValueSet/medication-form-codes,ValueSet/body-site,ValueSet/manifestation-or-symptom,ValueSet/procedure-code,ValueSet/goal-start-event,ValueSet/medication-as-needed-reason,ValueSet/c80-facilitycodes,ValueSet/immunization-reason,ValueSet/substance-code,ValueSet/simple-observation,ValueSet/care-plan-category,ValueSet/us-core-procedure-code,ValueSet/observation-methods,ValueSet/questionnaire-answers,ValueSet/servicerequest-orderdetail,ValueSet/clinical-findings,ValueSet/us-core-encounter-type,ValueSet/condition-stage,ValueSet/encounter-reason,ValueSet/us-core-observation-smokingstatus-max,ValueSet/immunization-target-disease,ValueSet/participant-role,ValueSet/additional-instruction-codes,ValueSet/us-core-observation-value-codes,ValueSet/approach-site-codes,ValueSet/device-action,ValueSet/us-core-condition-code,ValueSet/us-core-sexual-orientation,ValueSet/medication-codes,ValueSet/device-kind,ValueSet/performer-role,ValueSet/us-core-servicerequest-category,ValueSet/c80-practice-codes,ValueSet/referencerange-appliesto,ValueSet/route-codes,ValueSet/procedure-outcome,ValueSet/care-plan-activity-outcome,ValueSet/procedure-category,ValueSet/condition-code,ValueSet/condition-stage-type,ValueSet/immunization-status-reason,ValueSet/procedure-not-performed-reason,ValueSet/administration-method-codes,ValueSet/condition-severity</t>
+          <t>ValueSet/2.16.840.1.114222.4.11.7900,ValueSet/2.16.840.1.114222.4.11.7901</t>
         </is>
       </c>
       <c r="I53" t="inlineStr"/>
@@ -2747,42 +2763,42 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/PHOccupationalDataForHealthODH</t>
+          <t>http://terminology.hl7.org/CodeSystem/admit-source</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>2.0.1</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>2.16.840.1.114222.4.5.327</t>
+          <t>2.16.840.1.113883.4.642.1.1092</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>PHOccupationalDataForHealthODH</t>
+          <t>AdmitSource</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Occupational Data for Health (ODH)</t>
+          <t>Admit source</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>The concepts representing the values supporting Occupational Data for Health, including Job Supervisory Level or Pay Grade (ODH) code system consists of data elements that describe a person's work information, structured to facilitate individual, population, and public health use; not intended to support billing.).</t>
+          <t>This value set defines a set of codes that can be used to indicate from where the patient came in.</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>ValueSet/2.16.840.1.114222.4.11.7900,ValueSet/2.16.840.1.114222.4.11.7901</t>
+          <t>ValueSet/encounter-admit-source</t>
         </is>
       </c>
       <c r="I54" t="inlineStr"/>
@@ -2791,12 +2807,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/admit-source</t>
+          <t>http://terminology.hl7.org/CodeSystem/allergyintolerance-clinical</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>0.1.0</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2806,27 +2822,27 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1092</t>
+          <t>2.16.840.1.113883.4.642.1.1373</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>AdmitSource</t>
+          <t>AllergyIntoleranceClinicalStatusCodes</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Admit source</t>
+          <t>AllergyIntolerance Clinical Status Codes</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>This value set defines a set of codes that can be used to indicate from where the patient came in.</t>
+          <t>Preferred value set for AllergyIntolerance Clinical Status.</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>ValueSet/encounter-admit-source</t>
+          <t>ValueSet/allergyintolerance-clinical</t>
         </is>
       </c>
       <c r="I55" t="inlineStr"/>
@@ -2835,12 +2851,12 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/allergyintolerance-clinical</t>
+          <t>http://terminology.hl7.org/CodeSystem/allergyintolerance-verification</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>0.5.0</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2850,27 +2866,27 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1373</t>
+          <t>2.16.840.1.113883.4.642.1.1371</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>AllergyIntoleranceClinicalStatusCodes</t>
+          <t>AllergyIntoleranceVerificationStatus</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>AllergyIntolerance Clinical Status Codes</t>
+          <t>AllergyIntolerance Verification Status</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Preferred value set for AllergyIntolerance Clinical Status.</t>
+          <t>The verification status to support or decline the clinical status of the allergy or intolerance.</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>ValueSet/allergyintolerance-clinical</t>
+          <t>ValueSet/allergyintolerance-verification</t>
         </is>
       </c>
       <c r="I56" t="inlineStr"/>
@@ -2879,12 +2895,12 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/allergyintolerance-verification</t>
+          <t>http://terminology.hl7.org/CodeSystem/common-tags</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>0.5.0</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2894,27 +2910,27 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1371</t>
+          <t>2.16.840.1.113883.4.642.1.1067</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>AllergyIntoleranceVerificationStatus</t>
+          <t>CommonTags</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>AllergyIntolerance Verification Status</t>
+          <t>Common Tags</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>The verification status to support or decline the clinical status of the allergy or intolerance.</t>
+          <t>Common Tag Codes defined by FHIR project</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>ValueSet/allergyintolerance-verification</t>
+          <t>ValueSet/common-tags</t>
         </is>
       </c>
       <c r="I57" t="inlineStr"/>
@@ -2928,7 +2944,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>0.5.0</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2972,7 +2988,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>2.0.0</t>
+          <t>3.0.0</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -3016,7 +3032,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>1.0.0</t>
+          <t>2.0.0</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -3060,7 +3076,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>0.5.0</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -3104,7 +3120,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>0.1.0</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -3148,7 +3164,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>0.1.0</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -3192,7 +3208,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>0.1.0</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -3236,7 +3252,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>0.1.0</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -3280,7 +3296,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>0.1.0</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -3324,7 +3340,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>0.1.1</t>
+          <t>1.1.0</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -3368,7 +3384,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>0.1.0</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -3412,7 +3428,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>0.1.0</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -3456,7 +3472,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>0.1.0</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -3500,7 +3516,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>0.1.0</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -3544,7 +3560,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>0.2.0</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -3584,7 +3600,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>0.1.0</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -3628,7 +3644,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>0.1.0</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -3672,7 +3688,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>0.1.0</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -3716,7 +3732,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>0.1.0</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -3760,7 +3776,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>0.1.0</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -3804,7 +3820,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>0.1.0</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -3848,7 +3864,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>0.1.0</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -3892,7 +3908,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>1.0.0</t>
+          <t>2.0.0</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3936,7 +3952,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>0.1.0</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -4024,7 +4040,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>0.1.0</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -4068,7 +4084,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>0.1.0</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -4112,7 +4128,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>0.1.0</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -4156,7 +4172,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>0.1.0</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -4200,7 +4216,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>0.1.0</t>
+          <t>2.0.0</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -4244,7 +4260,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>0.5.0</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -4288,7 +4304,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>0.1.0</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -4318,7 +4334,7 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>ValueSet/provenance-agent-type,ValueSet/us-core-provenance-participant-type</t>
+          <t>ValueSet/provenance-agent-type</t>
         </is>
       </c>
       <c r="I89" t="inlineStr"/>
@@ -4332,7 +4348,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>0.1.0</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -4376,7 +4392,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>0.1.0</t>
+          <t>1.1.0</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -4420,7 +4436,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>0.1.0</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -4640,7 +4656,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>3.0.0</t>
+          <t>4.0.0</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -4904,7 +4920,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>8.0.1</t>
+          <t>9.0.0</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -4948,7 +4964,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>2.1.0</t>
+          <t>3.0.0</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -4992,7 +5008,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>2.1.1</t>
+          <t>3.0.0</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -5036,7 +5052,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>2.1.0</t>
+          <t>3.0.0</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -5080,7 +5096,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>4.1.0</t>
+          <t>5.0.0</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -5124,7 +5140,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>2.1.0</t>
+          <t>3.0.0</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -5168,7 +5184,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>2.1.0</t>
+          <t>3.0.0</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -5207,12 +5223,12 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v3-MaritalStatus</t>
+          <t>http://terminology.hl7.org/CodeSystem/v3-HL7DocumentFormatCodes</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>2.1.0</t>
+          <t>4.0.0</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -5222,27 +5238,27 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.5.2</t>
+          <t>2.16.840.1.113883.4.642.1.1407</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>MaritalStatus</t>
+          <t>HL7DocumentFormatCodes</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>MaritalStatus</t>
+          <t>HL7 Document Format Codes</t>
         </is>
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>\* \* \* No description supplied \* \* \*    *Open Issue:* The specific meanings of these codes can vary somewhat by jurisdiction and implementation so caution should be used when determining equivalency.    *Open Issue:* fixing and completion of the hierarchy and proper good definitions of all the concepts is badly needed.</t>
+          <t>This codeSystem contains codes which specify the technical format of a document. Each code provides sufficient information to allow any potential document consumer to know if it will be able to process the document. The codes are sufficiently specific to ensure processing/display by identifying a document encoding, structure and template. For example, formatCodes can be used in the FHIR DocumentReference resource to characterize the document being referenced.</t>
         </is>
       </c>
       <c r="H110" t="inlineStr">
         <is>
-          <t>ValueSet/marital-status</t>
+          <t>ValueSet/v3-HL7FormatCodes</t>
         </is>
       </c>
       <c r="I110" t="inlineStr"/>
@@ -5251,12 +5267,12 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v3-NullFlavor</t>
+          <t>http://terminology.hl7.org/CodeSystem/v3-MaritalStatus</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>2.1.0</t>
+          <t>3.0.0</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -5266,27 +5282,27 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.5.1008</t>
+          <t>2.16.840.1.113883.5.2</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>NullFlavor</t>
+          <t>MaritalStatus</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>NullFlavor</t>
+          <t>MaritalStatus</t>
         </is>
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>A collection of codes specifying why a valid value is not present.</t>
+          <t>\* \* \* No description supplied \* \* \*    *Open Issue:* The specific meanings of these codes can vary somewhat by jurisdiction and implementation so caution should be used when determining equivalency.    *Open Issue:* fixing and completion of the hierarchy and proper good definitions of all the concepts is badly needed.</t>
         </is>
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>ValueSet/us-core-documentreference-type,ValueSet/us-core-sexual-orientation,ValueSet/us-core-pregnancy-intent,ValueSet/marital-status,ValueSet/us-core-pregnancy-status,ValueSet/encounter-special-courtesy</t>
+          <t>ValueSet/marital-status</t>
         </is>
       </c>
       <c r="I111" t="inlineStr"/>
@@ -5295,12 +5311,12 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v3-ObservationInterpretation</t>
+          <t>http://terminology.hl7.org/CodeSystem/v3-NullFlavor</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>2.1.0</t>
+          <t>3.0.0</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -5310,27 +5326,27 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.5.83</t>
+          <t>2.16.840.1.113883.5.1008</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>ObservationInterpretation</t>
+          <t>NullFlavor</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>ObservationInterpretation</t>
+          <t>NullFlavor</t>
         </is>
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>One or more codes providing a rough qualitative interpretation of the observation, such as "normal" / "abnormal", "low" / "high", "better" / "worse", "resistant" / "susceptible", "expected" / "not expected". The value set is intended to be for ANY use where coded representation of an interpretation is needed.</t>
+          <t>A collection of codes specifying why a valid value is not present.</t>
         </is>
       </c>
       <c r="H112" t="inlineStr">
         <is>
-          <t>ValueSet/observation-interpretation</t>
+          <t>ValueSet/us-core-documentreference-type,ValueSet/us-core-pregnancy-intent,ValueSet/marital-status,ValueSet/encounter-special-courtesy,ValueSet/us-core-pregnancy-status</t>
         </is>
       </c>
       <c r="I112" t="inlineStr"/>
@@ -5339,12 +5355,12 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v3-ParticipationFunction</t>
+          <t>http://terminology.hl7.org/CodeSystem/v3-ObservationInterpretation</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>2.1.0</t>
+          <t>3.0.0</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -5354,27 +5370,27 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.5.88</t>
+          <t>2.16.840.1.113883.5.83</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>ParticipationFunction</t>
+          <t>ObservationInterpretation</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>ParticipationFunction</t>
+          <t>ObservationInterpretation</t>
         </is>
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>This code is used to specify the exact function an actor had in a service in all necessary detail. This domain may include local extensions (CWE).</t>
+          <t>One or more codes providing a rough qualitative interpretation of the observation, such as "normal" / "abnormal", "low" / "high", "better" / "worse", "resistant" / "susceptible", "expected" / "not expected". The value set is intended to be for ANY use where coded representation of an interpretation is needed.</t>
         </is>
       </c>
       <c r="H113" t="inlineStr">
         <is>
-          <t>ValueSet/security-role-type</t>
+          <t>ValueSet/observation-interpretation</t>
         </is>
       </c>
       <c r="I113" t="inlineStr"/>
@@ -5383,12 +5399,12 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v3-ParticipationType</t>
+          <t>http://terminology.hl7.org/CodeSystem/v3-ParticipationFunction</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>4.0.0</t>
+          <t>3.0.0</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -5398,27 +5414,27 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.5.90</t>
+          <t>2.16.840.1.113883.5.88</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>ParticipationType</t>
+          <t>ParticipationFunction</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>ParticipationType</t>
+          <t>ParticipationFunction</t>
         </is>
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>A code specifying the meaning and purpose of every Participation instance. Each of its values implies specific constraints on the Roles undertaking the participation.</t>
+          <t>This code is used to specify the exact function an actor had in a service in all necessary detail. This domain may include local extensions (CWE).</t>
         </is>
       </c>
       <c r="H114" t="inlineStr">
         <is>
-          <t>ValueSet/security-role-type,ValueSet/encounter-participant-type,ValueSet/provenance-activity-type</t>
+          <t>ValueSet/security-role-type</t>
         </is>
       </c>
       <c r="I114" t="inlineStr"/>
@@ -5427,12 +5443,12 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v3-RoleClass</t>
+          <t>http://terminology.hl7.org/CodeSystem/v3-ParticipationType</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>3.1.0</t>
+          <t>5.0.0</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -5442,27 +5458,27 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.5.110</t>
+          <t>2.16.840.1.113883.5.90</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>RoleClass</t>
+          <t>ParticipationType</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>RoleClass</t>
+          <t>ParticipationType</t>
         </is>
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>Codes for the Role class hierarchy. The values in this hierarchy, represent a Role which is an association or relationship between two entities - the entity that plays the role and the entity that scopes the role. Roles names are derived from the name of the playing entity in that role.    The role hierarchy stems from three core concepts, or abstract domains:     *  **RoleClassOntological** is an abstract domain that collects roles in which the playing entity is defined or specified by the scoping entity.   *  **RoleClassPartitive** collects roles in which the playing entity is in some sense a "part" of the scoping entity.   *  **RoleClassAssociative** collects all of the remaining forms of association between the playing entity and the scoping entity. This set of roles is further partitioned between:             *  **RoleClassPassive** which are roles in which the playing entity is used, known, treated, handled, built, or destroyed, etc. under the auspices of the scoping entity. The playing entity is passive in these roles in that the role exists without an agreement from the playing entity.       *  **RoleClassMutualRelationship** which are relationships based on mutual behavior of the two entities. The basis of these relationship may be formal agreements or they may be *de facto* behavior. Thus, this sub-domain is further divided into:                     *  **RoleClassRelationshipFormal** in which the relationship is formally defined, frequently by a contract or agreement.           *  **Personal relationship** which inks two people in a personal relationship.    The hierarchy discussed above is represented In the current vocabulary tables as a set of abstract domains, with the exception of the "Personal relationship" which is a leaf concept.    *OpenIssue:* Description copied from Concept Domain of same name. Must be verified.</t>
+          <t>A code specifying the meaning and purpose of every Participation instance. Each of its values implies specific constraints on the Roles undertaking the participation.</t>
         </is>
       </c>
       <c r="H115" t="inlineStr">
         <is>
-          <t>ValueSet/security-role-type</t>
+          <t>ValueSet/security-role-type,ValueSet/encounter-participant-type,ValueSet/provenance-activity-type</t>
         </is>
       </c>
       <c r="I115" t="inlineStr"/>
@@ -5471,12 +5487,12 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v3-RoleCode</t>
+          <t>http://terminology.hl7.org/CodeSystem/v3-RoleClass</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>2.2.0</t>
+          <t>4.0.0</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -5486,27 +5502,27 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.5.111</t>
+          <t>2.16.840.1.113883.5.110</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>RoleCode</t>
+          <t>RoleClass</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>RoleCode</t>
+          <t>RoleClass</t>
         </is>
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>A set of codes further specifying the kind of Role; specific classification codes for further qualifying RoleClass codes.</t>
+          <t>Codes for the Role class hierarchy. The values in this hierarchy, represent a Role which is an association or relationship between two entities - the entity that plays the role and the entity that scopes the role. Roles names are derived from the name of the playing entity in that role.    The role hierarchy stems from three core concepts, or abstract domains:     *  **RoleClassOntological** is an abstract domain that collects roles in which the playing entity is defined or specified by the scoping entity.   *  **RoleClassPartitive** collects roles in which the playing entity is in some sense a "part" of the scoping entity.   *  **RoleClassAssociative** collects all of the remaining forms of association between the playing entity and the scoping entity. This set of roles is further partitioned between:             *  **RoleClassPassive** which are roles in which the playing entity is used, known, treated, handled, built, or destroyed, etc. under the auspices of the scoping entity. The playing entity is passive in these roles in that the role exists without an agreement from the playing entity.       *  **RoleClassMutualRelationship** which are relationships based on mutual behavior of the two entities. The basis of these relationship may be formal agreements or they may be *de facto* behavior. Thus, this sub-domain is further divided into:                     *  **RoleClassRelationshipFormal** in which the relationship is formally defined, frequently by a contract or agreement.           *  **Personal relationship** which inks two people in a personal relationship.    The hierarchy discussed above is represented In the current vocabulary tables as a set of abstract domains, with the exception of the "Personal relationship" which is a leaf concept.    *OpenIssue:* Description copied from Concept Domain of same name. Must be verified.</t>
         </is>
       </c>
       <c r="H116" t="inlineStr">
         <is>
-          <t>ValueSet/security-role-type,ValueSet/relatedperson-relationshiptype,ValueSet/v3-ServiceDeliveryLocationRoleType</t>
+          <t>ValueSet/security-role-type</t>
         </is>
       </c>
       <c r="I116" t="inlineStr"/>
@@ -5515,12 +5531,12 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v3-RouteOfAdministration</t>
+          <t>http://terminology.hl7.org/CodeSystem/v3-RoleCode</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>2.1.0</t>
+          <t>3.0.0</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -5530,27 +5546,27 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.5.112</t>
+          <t>2.16.840.1.113883.5.111</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>RouteOfAdministration</t>
+          <t>RoleCode</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>RouteOfAdministration</t>
+          <t>RoleCode</t>
         </is>
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>The path the administered medication takes to get into the body or into contact with the body.</t>
+          <t>A set of codes further specifying the kind of Role; specific classification codes for further qualifying RoleClass codes.</t>
         </is>
       </c>
       <c r="H117" t="inlineStr">
         <is>
-          <t>ValueSet/immunization-route</t>
+          <t>ValueSet/security-role-type,ValueSet/relatedperson-relationshiptype,ValueSet/v3-ServiceDeliveryLocationRoleType</t>
         </is>
       </c>
       <c r="I117" t="inlineStr"/>
@@ -5559,7 +5575,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v3-TribalEntityUS</t>
+          <t>http://terminology.hl7.org/CodeSystem/v3-RouteOfAdministration</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -5574,27 +5590,27 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.5.140</t>
+          <t>2.16.840.1.113883.5.112</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>TribalEntityUS</t>
+          <t>RouteOfAdministration</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>TribalEntityUS</t>
+          <t>RouteOfAdministration</t>
         </is>
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>INDIAN ENTITIES RECOGNIZED AND ELIGIBLE TO RECEIVE SERVICES FROM THE UNITED STATES BUREAU OF INDIAN AFFAIRS</t>
+          <t>The path the administered medication takes to get into the body or into contact with the body.</t>
         </is>
       </c>
       <c r="H118" t="inlineStr">
         <is>
-          <t>ValueSet/v3-TribalEntityUS</t>
+          <t>ValueSet/immunization-route</t>
         </is>
       </c>
       <c r="I118" t="inlineStr"/>
@@ -5603,12 +5619,12 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v3-substanceAdminSubstitution</t>
+          <t>http://terminology.hl7.org/CodeSystem/v3-TribalEntityUS</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>2.1.0</t>
+          <t>4.0.0</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -5618,27 +5634,27 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.5.1070</t>
+          <t>2.16.840.1.113883.5.140</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>SubstanceAdminSubstitution</t>
+          <t>TribalEntityUS</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>Substance Admin Substitution</t>
+          <t>TribalEntityUS</t>
         </is>
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>Identifies what sort of change is permitted or has occurred between the therapy that was ordered and the therapy that was/will be provided.</t>
+          <t>INDIAN ENTITIES RECOGNIZED AND ELIGIBLE TO RECEIVE SERVICES FROM THE UNITED STATES BUREAU OF INDIAN AFFAIRS</t>
         </is>
       </c>
       <c r="H119" t="inlineStr">
         <is>
-          <t>ValueSet/v3-ActSubstanceAdminSubstitutionCode</t>
+          <t>ValueSet/v3-TribalEntityUS</t>
         </is>
       </c>
       <c r="I119" t="inlineStr"/>
@@ -5647,42 +5663,42 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/fhir/CodeSystem/medicationdispense-category</t>
+          <t>http://terminology.hl7.org/CodeSystem/v3-substanceAdminSubstitution</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>4.0.1</t>
+          <t>3.0.0</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>draft</t>
+          <t>active</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.4.1315</t>
+          <t>2.16.840.1.113883.5.1070</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>MedicationDispense Category Codes</t>
+          <t>SubstanceAdminSubstitution</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>Medication dispense  category  codes</t>
+          <t>Substance Admin Substitution</t>
         </is>
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>MedicationDispense Category Codes</t>
+          <t>Identifies what sort of change is permitted or has occurred between the therapy that was ordered and the therapy that was/will be provided.</t>
         </is>
       </c>
       <c r="H120" t="inlineStr">
         <is>
-          <t>ValueSet/medicationdispense-category</t>
+          <t>ValueSet/v3-ActSubstanceAdminSubstitutionCode</t>
         </is>
       </c>
       <c r="I120" t="inlineStr"/>
@@ -5691,7 +5707,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/fhir/CodeSystem/medicationdispense-status-reason</t>
+          <t>http://terminology.hl7.org/fhir/CodeSystem/medicationdispense-category</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -5706,27 +5722,27 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.4.1317</t>
+          <t>2.16.840.1.113883.4.642.4.1315</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>MedicationDispense Status Reason Codes</t>
+          <t>MedicationDispense Category Codes</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>Medication dispense  status  reason  codes</t>
+          <t>Medication dispense  category  codes</t>
         </is>
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>MedicationDispense Status Codes</t>
+          <t>MedicationDispense Category Codes</t>
         </is>
       </c>
       <c r="H121" t="inlineStr">
         <is>
-          <t>ValueSet/medicationdispense-status-reason</t>
+          <t>ValueSet/medicationdispense-category</t>
         </is>
       </c>
       <c r="I121" t="inlineStr"/>
@@ -5735,42 +5751,42 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>http://unitsofmeasure.org</t>
+          <t>http://terminology.hl7.org/fhir/CodeSystem/medicationdispense-status-reason</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>3.0.1</t>
+          <t>4.0.1</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.6.8</t>
+          <t>2.16.840.1.113883.4.642.4.1317</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>UCUM</t>
+          <t>MedicationDispense Status Reason Codes</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>Unified Code for Units of Measure (UCUM)</t>
+          <t>Medication dispense  status  reason  codes</t>
         </is>
       </c>
       <c r="G122" t="inlineStr">
         <is>
-          <t>The Unified Code for Units of Measure (UCUM) is a code system intended to include all units of measures being contemporarily used in international science, engineering, and business. The purpose is to facilitate unambiguous electronic communication of quantities together with their units. The focus is on electronic communication, as opposed to communication between humans. A typical application of The Unified Code for Units of Measure are electronic data interchange (EDI) protocols, but there is nothing that prevents it from being used in other types of machine communication.</t>
+          <t>MedicationDispense Status Codes</t>
         </is>
       </c>
       <c r="H122" t="inlineStr">
         <is>
-          <t>ValueSet/ucum-bodyweight,ValueSet/ucum-bodytemp,ValueSet/ucum-common,ValueSet/ucum-vitals-common,ValueSet/ucum-bodylength</t>
+          <t>ValueSet/medicationdispense-status-reason</t>
         </is>
       </c>
       <c r="I122" t="inlineStr"/>
@@ -5779,7 +5795,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>http://www.ada.org/cdt</t>
+          <t>http://unitsofmeasure.org</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -5794,27 +5810,27 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.6.13</t>
+          <t>2.16.840.1.113883.6.8</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>CDT</t>
+          <t>UCUM</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>Code on Dental Procedures and Nomenclature</t>
+          <t>Unified Code for Units of Measure (UCUM)</t>
         </is>
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>The purpose of the CDT Code is to achieve uniformity, consistency and specificity in accurately documenting dental treatment. One use of the CDT Code is to provide for the efficient processing of dental claims, and another is to populate an Electronic Health Record.</t>
+          <t>The Unified Code for Units of Measure (UCUM) is a code system intended to include all units of measures being contemporarily used in international science, engineering, and business. The purpose is to facilitate unambiguous electronic communication of quantities together with their units. The focus is on electronic communication, as opposed to communication between humans. A typical application of The Unified Code for Units of Measure are electronic data interchange (EDI) protocols, but there is nothing that prevents it from being used in other types of machine communication.</t>
         </is>
       </c>
       <c r="H123" t="inlineStr">
         <is>
-          <t>ValueSet/us-core-procedure-code</t>
+          <t>ValueSet/ucum-bodyweight,ValueSet/ucum-bodytemp,ValueSet/ucum-common,ValueSet/ucum-vitals-common,ValueSet/ucum-bodylength,ValueSet/v3-UnitsOfMeasureCaseSensitive</t>
         </is>
       </c>
       <c r="I123" t="inlineStr"/>
@@ -5823,7 +5839,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>http://www.ama-assn.org/go/cpt</t>
+          <t>http://www.ada.org/cdt</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -5838,27 +5854,27 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.6.12</t>
+          <t>2.16.840.1.113883.6.13</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>CPT</t>
+          <t>CDT</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>Current Procedural Terminology (CPT®)</t>
+          <t>Code on Dental Procedures and Nomenclature</t>
         </is>
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>The Current Procedural Terminology (CPT) code set, created and maintained by the American Medical Association, is the language of medicine today and the code to its future. This system of terminology is the most widely accepted medical nomenclature used to report medical procedures and services under public and private health insurance programs. CPT coding is also used for administrative management purposes such as claims processing and developing guidelines for medical care review. Each year, via a rigorous, evidence-based and transparent process, the independent CPT Editorial Panel revises, creates or deletes hundreds of codes in order to reflect current medical practice.    Designated by the U.S. Department of Health and Human Services under the Health Insurance Portability and Accountability Act (HIPAA) as a national coding set for physician and other health care professional services and procedures, CPT’s evidence-based codes accurately encompass the full range of health care services.    All CPT codes are five-digits and can be either numeric or alphanumeric, depending on the category. CPT code descriptors are clinically focused and utilize common standards so that a diverse set of users can have common understanding across the clinical health care paradigm.    There are various types of CPT codes:    Category I: These codes have descriptors that correspond to a procedure or service. Codes range from 00100–99499 and are generally ordered into sub-categories based on procedure/service type and anatomy.    Category II: These alphanumeric tracking codes are supplemental codes used for performance measurement. Using them is optional and not required for correct coding.    Category III: These are temporary alphanumeric codes for new and developing technology, procedures and services. They were created for data collection, assessment and in some instances, payment of new services and procedures that currently don’t meet the criteria for a Category I code.    Proprietary Laboratory Analyses (PLA) codes: These codes describe proprietary clinical laboratory analyses and can be either provided by a single (“solesource”) laboratory or licensed or marketed to multiple providing laboratories that are cleared or approved by the Food and Drug Administration (FDA)). This category includes but is not limited to Advanced Diagnostic Laboratory Tests (ADLTs) and Clinical Diagnostic Laboratory Tests (CDLTs), as defined under the Protecting Access to Medicare Act of 2014 (PAMA).</t>
+          <t>The purpose of the CDT Code is to achieve uniformity, consistency and specificity in accurately documenting dental treatment. One use of the CDT Code is to provide for the efficient processing of dental claims, and another is to populate an Electronic Health Record.</t>
         </is>
       </c>
       <c r="H124" t="inlineStr">
         <is>
-          <t>ValueSet/us-core-encounter-type,ValueSet/us-core-procedure-code</t>
+          <t>ValueSet/us-core-procedure-code</t>
         </is>
       </c>
       <c r="I124" t="inlineStr"/>
@@ -5867,12 +5883,12 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>http://www.cms.gov/Medicare/Coding/ICD10</t>
+          <t>http://www.ama-assn.org/go/cpt</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>2.0.1</t>
+          <t>3.0.1</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -5882,27 +5898,27 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.6.4</t>
+          <t>2.16.840.1.113883.6.12</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>Icd10PCS</t>
+          <t>CPT</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>ICD-10 Procedure Codes</t>
+          <t>Current Procedural Terminology (CPT®)</t>
         </is>
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>ICD Procedure Coding System (ICD 10 PCS)</t>
+          <t>The Current Procedural Terminology (CPT) code set, created and maintained by the American Medical Association, is the language of medicine today and the code to its future. This system of terminology is the most widely accepted medical nomenclature used to report medical procedures and services under public and private health insurance programs. CPT coding is also used for administrative management purposes such as claims processing and developing guidelines for medical care review. Each year, via a rigorous, evidence-based and transparent process, the independent CPT Editorial Panel revises, creates or deletes hundreds of codes in order to reflect current medical practice.    Designated by the U.S. Department of Health and Human Services under the Health Insurance Portability and Accountability Act (HIPAA) as a national coding set for physician and other health care professional services and procedures, CPT’s evidence-based codes accurately encompass the full range of health care services.    All CPT codes are five-digits and can be either numeric or alphanumeric, depending on the category. CPT code descriptors are clinically focused and utilize common standards so that a diverse set of users can have common understanding across the clinical health care paradigm.    There are various types of CPT codes:    Category I: These codes have descriptors that correspond to a procedure or service. Codes range from 00100–99499 and are generally ordered into sub-categories based on procedure/service type and anatomy.    Category II: These alphanumeric tracking codes are supplemental codes used for performance measurement. Using them is optional and not required for correct coding.    Category III: These are temporary alphanumeric codes for new and developing technology, procedures and services. They were created for data collection, assessment and in some instances, payment of new services and procedures that currently don’t meet the criteria for a Category I code.    Proprietary Laboratory Analyses (PLA) codes: These codes describe proprietary clinical laboratory analyses and can be either provided by a single (“solesource”) laboratory or licensed or marketed to multiple providing laboratories that are cleared or approved by the Food and Drug Administration (FDA)). This category includes but is not limited to Advanced Diagnostic Laboratory Tests (ADLTs) and Clinical Diagnostic Laboratory Tests (CDLTs), as defined under the Protecting Access to Medicare Act of 2014 (PAMA).</t>
         </is>
       </c>
       <c r="H125" t="inlineStr">
         <is>
-          <t>ValueSet/us-core-procedure-code</t>
+          <t>ValueSet/us-core-encounter-type,ValueSet/us-core-procedure-code</t>
         </is>
       </c>
       <c r="I125" t="inlineStr"/>
@@ -5911,32 +5927,42 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>https://nahdo.org/sopt</t>
-        </is>
-      </c>
-      <c r="B126" t="n">
-        <v>9.199999999999999</v>
+          <t>http://www.cms.gov/Medicare/Coding/ICD10</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>2.0.1</t>
+        </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
           <t>active</t>
         </is>
       </c>
-      <c r="D126" t="inlineStr"/>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>2.16.840.1.113883.6.4</t>
+        </is>
+      </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>SOP</t>
+          <t>Icd10PCS</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>Source of Payment Typology</t>
-        </is>
-      </c>
-      <c r="G126" t="inlineStr"/>
+          <t>ICD-10 Procedure Codes</t>
+        </is>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>ICD Procedure Coding System (ICD 10 PCS)</t>
+        </is>
+      </c>
       <c r="H126" t="inlineStr">
         <is>
-          <t>ValueSet/2.16.840.1.114222.4.11.3591</t>
+          <t>ValueSet/us-core-procedure-code</t>
         </is>
       </c>
       <c r="I126" t="inlineStr"/>
@@ -5945,42 +5971,32 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>https://www.cms.gov/Medicare/Coding/HCPCSReleaseCodeSets</t>
-        </is>
-      </c>
-      <c r="B127" t="inlineStr">
-        <is>
-          <t>1.0.1</t>
-        </is>
+          <t>https://nahdo.org/sopt</t>
+        </is>
+      </c>
+      <c r="B127" t="n">
+        <v>9.199999999999999</v>
       </c>
       <c r="C127" t="inlineStr">
         <is>
           <t>active</t>
         </is>
       </c>
-      <c r="D127" t="inlineStr">
-        <is>
-          <t>2.16.840.1.113883.6.285</t>
-        </is>
-      </c>
+      <c r="D127" t="inlineStr"/>
       <c r="E127" t="inlineStr">
         <is>
-          <t>HCPCSLevelII</t>
+          <t>SOP</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>Healthcare Common Procedure Coding System (HCPCS) level II alphanumeric codes</t>
-        </is>
-      </c>
-      <c r="G127" t="inlineStr">
-        <is>
-          <t>The Level II HCPCS codes, which are established by CMS's Alpha-Numeric Editorial Panel, primarily represent items and supplies and non-physician services not covered by the American Medical Association's Current Procedural Terminology-4 (CPT-4) codes; Medicare, Medicaid, and private health insurers use HCPCS procedure and modifier codes for claims processing.  Level II alphanumeric procedure and modifier codes comprise the A to V range.</t>
-        </is>
-      </c>
+          <t>Source of Payment Typology</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr"/>
       <c r="H127" t="inlineStr">
         <is>
-          <t>ValueSet/us-core-procedure-code</t>
+          <t>ValueSet/2.16.840.1.114222.4.11.3591</t>
         </is>
       </c>
       <c r="I127" t="inlineStr"/>
@@ -5989,12 +6005,12 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>urn:ietf:bcp:47</t>
+          <t>https://www.cms.gov/Medicare/Coding/HCPCSReleaseCodeSets</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>2.0.1</t>
+          <t>1.0.1</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -6004,31 +6020,119 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.6.121</t>
+          <t>2.16.840.1.113883.6.285</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>Ietf3066</t>
+          <t>HCPCSLevelII</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>Tags for the Identification of Languages</t>
+          <t>Healthcare Common Procedure Coding System (HCPCS) level II alphanumeric codes</t>
         </is>
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>Older value from OID registry.  Superceded; see recommendations in BCP-47.</t>
+          <t>The Level II HCPCS codes, which are established by CMS's Alpha-Numeric Editorial Panel, primarily represent items and supplies and non-physician services not covered by the American Medical Association's Current Procedural Terminology-4 (CPT-4) codes; Medicare, Medicaid, and private health insurers use HCPCS procedure and modifier codes for claims processing.  Level II alphanumeric procedure and modifier codes comprise the A to V range.</t>
         </is>
       </c>
       <c r="H128" t="inlineStr">
         <is>
-          <t>ValueSet/languages,ValueSet/simple-language</t>
+          <t>ValueSet/us-core-procedure-code</t>
         </is>
       </c>
       <c r="I128" t="inlineStr"/>
       <c r="J128" t="inlineStr"/>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>https://www.nubc.org/CodeSystem/PatDischargeStatus</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>1.0.0</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>2.16.840.1.113883.6.301.5</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>AHA_NUBC_PatientDischargeStatus</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>AHA NUBC Patient Discharge Status Codes</t>
+        </is>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>"The UB-04 Data File contains the complete set of NUBC codes. Every code in the range of possible codes is accounted for sequentially. There are no gaps because all used and unused codes are identified."    This code system consists of the following:    \* FL 17 - Patient Discharge Status    These codes are used to convey the patient discharge status and are the property of the American Hospital Association.    To obtain the underlying code systems, please see information [here](https://www.nubc.org/subscription-information)    Statement of Understanding between AHA and HL7 can be found [here](http://www.hl7.org/documentcenter/public/mou/AHA%20HL7%20SOU%202020%20AHA%20Fully%20Executed.pdf). In particular see sections 4.1d and 4.2.    "The UB-04 Manual has a 12-month subscription period from June 30 through July 1."    For frequently asked questions, see here [here](https://www.nubc.org/nubc-faqs)</t>
+        </is>
+      </c>
+      <c r="H129" t="inlineStr">
+        <is>
+          <t>ValueSet/us-core-discharge-disposition</t>
+        </is>
+      </c>
+      <c r="I129" t="inlineStr"/>
+      <c r="J129" t="inlineStr"/>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>urn:ietf:bcp:47</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>2.0.1</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>2.16.840.1.113883.6.121</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>Ietf3066</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>Tags for the Identification of Languages</t>
+        </is>
+      </c>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>Older value from OID registry.  Superceded; see recommendations in BCP-47.</t>
+        </is>
+      </c>
+      <c r="H130" t="inlineStr">
+        <is>
+          <t>ValueSet/languages,ValueSet/simple-language</t>
+        </is>
+      </c>
+      <c r="I130" t="inlineStr"/>
+      <c r="J130" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
fix open markdown links - update How to read this guide section
</commit_message>
<xml_diff>
--- a/input/images/tables/codesystem-ref-all-list.xlsx
+++ b/input/images/tables/codesystem-ref-all-list.xlsx
@@ -2268,7 +2268,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>4.0.1</t>
+          <t>4.0.0</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2352,7 +2352,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>ValueSet/us-core-condition-code</t>
+          <t>ValueSet/us-core-condition-code-current,ValueSet/us-core-condition-code</t>
         </is>
       </c>
     </row>
@@ -2452,7 +2452,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>8.0.0-ballot</t>
+          <t>8.0.0</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2496,7 +2496,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>8.0.0-ballot</t>
+          <t>8.0.0</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2526,7 +2526,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>ValueSet/us-core-screening-assessment-observation-category,ValueSet/us-core-simple-observation-category,ValueSet/us-core-servicerequest-category,ValueSet/us-core-screening-assessment-condition-category,ValueSet/us-core-screening-assessment-observation-maximum-category</t>
+          <t>ValueSet/us-core-screening-assessment-observation-category,ValueSet/us-core-simple-observation-category,ValueSet/us-core-screening-assessment-condition-category,ValueSet/us-core-servicerequest-category,ValueSet/us-core-screening-assessment-observation-maximum-category</t>
         </is>
       </c>
       <c r="I48" t="inlineStr"/>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>8.0.0-ballot</t>
+          <t>8.0.0</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2584,7 +2584,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>8.0.0-ballot</t>
+          <t>8.0.0</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2623,12 +2623,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>http://loinc.org</t>
+          <t>http://ihe.net/fhir/ihe.formatcode.fhir/CodeSystem/formatcode</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>3.1.0</t>
+          <t>1.3.0</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2638,45 +2638,41 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.6.1</t>
+          <t>1.3.6.1.4.1.19376.1.2.3</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>LOINC</t>
+          <t>IHE_FormatCode_codesystem</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Logical Observation Identifiers</t>
+          <t>IHE Format Code set for use with Document Sharing</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Names and Codes (LOINC)</t>
+          <t>The [IHE](http://www.ihe.net) FormatCode code system with canonical URI of http://ihe.net/fhir/ihe.formatcode.fhir/CodeSystem/formatcode is defined to be the set of FormatCodes define by IHE, for use with [Document Sharing](https://profiles.ihe.net/ITI/HIE-Whitepaper/index.html). This code set additionally includes, as deprecated, format codes defined by [HL7 for some Implementation Guides](http://wiki.hl7.org/index.php?title=CDA_Format_Codes_for_IHE_XDS). The HL7 codes are now managed by HL7. The set of IHE FormatCode codes was listed in HITSP C80 Table 2-153 Format Code Value Set Definition, but since has been updated. The use of the FormatCode specifies the technical format of the document. The FormatCode tends to reference the IHE Content Profile (Implementation Guide) that defines the use-case and constraints. The FormatCode is a further specialization more detailed than the mime-type. The FormatCode provides sufficient metadata information to allow any potential document content consumer to know if it can process and/or display by identifying a document encoding, structure and template. The set of codes is intended to be preferred.</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>LOINC provides a set of universal names and ID codes for identifying laboratory and clinical test results.1,2 LOINC facilitates the exchange and pooling of results, such as blood hemoglobin, serum potassium, or vital signs, for clinical care, outcomes management, and research. LOINC's universal identifiers (names and codes) can be used in the context of order and observation exchanges between information systems that use syntax standards such as HL73, CEN TC251, ISO TC215, ASTM4, and DICOM. Specifically, the identifier can be used as the coded value for an observation in any other standard that uses the observation/observation value paradigm, whether messages, documents, application programming interface (API), etc. For example, LOINC codes are used widely in the OBX segment Observation Identifier field (OBX-3) of an ORU HL7 (HL7 version 2.x or ASTM 1238-9410) message that may be sent between a Clinical Laboratory Information Management Systems (LIMS) and Electronic Health Record Systems (EHR).5, 6 In this way, LOINC codes provide universal identifiers that allow the exchange of clinical data between heterogeneous computing environments.</t>
-        </is>
-      </c>
-      <c r="I51" t="inlineStr">
-        <is>
-          <t>ValueSet/us-core-diagnosticreport-category,ValueSet/c80-doc-typecodes,ValueSet/us-core-documentreference-type,ValueSet/document-classcodes,ValueSet/2.16.840.1.113883.3.88.12.80.62,ValueSet/2.16.840.1.113762.1.4.1267.13,ValueSet/us-core-clinical-note-type,ValueSet/us-core-laboratory-test-codes,ValueSet/us-core-goal-description,ValueSet/care-team-category,ValueSet/us-core-diagnosticreport-report-and-note-codes,ValueSet/observation-codes,ValueSet/us-core-procedure-code</t>
-        </is>
-      </c>
+          <t>ValueSet/v3-HL7FormatCodes</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr"/>
       <c r="J51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>http://snomed.info/sct</t>
+          <t>http://loinc.org</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>3.1.0</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2686,41 +2682,45 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.6.96</t>
+          <t>2.16.840.1.113883.6.1</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>SNOMED_CT</t>
+          <t>LOINC</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>SNOMED CT (all versions)</t>
+          <t>Logical Observation Identifiers</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>SNOMED CT is the most comprehensive and precise clinical health terminology product in the world, owned and distributed around the world by The International Health Terminology Standards Development Organisation (IHTSDO).</t>
+          <t xml:space="preserve"> Names and Codes (LOINC)</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>ValueSet/servicerequest-category,ValueSet/condition-stage,ValueSet/clinical-findings,ValueSet/immunization-target-disease,ValueSet/encounter-reason,ValueSet/specimen-container-type,ValueSet/additional-instruction-codes,ValueSet/participant-role,ValueSet/2.16.840.1.113762.1.4.1099.54,ValueSet/approach-site-codes,ValueSet/procedure-followup,ValueSet/us-core-goal-description,ValueSet/device-action,ValueSet/specimen-collection-method,ValueSet/medication-form-codes,ValueSet/us-core-condition-code,ValueSet/medication-codes,ValueSet/body-site,ValueSet/manifestation-or-symptom,ValueSet/goal-start-event,ValueSet/procedure-code,ValueSet/medication-as-needed-reason,ValueSet/2.16.840.1.113762.1.4.1166.22,ValueSet/device-kind,ValueSet/performer-role,ValueSet/c80-facilitycodes,ValueSet/immunization-reason,ValueSet/2.16.840.1.113762.1.4.1267.3,ValueSet/c80-practice-codes,ValueSet/referencerange-appliesto,ValueSet/us-core-servicerequest-category,ValueSet/route-codes,ValueSet/substance-code,ValueSet/procedure-outcome,ValueSet/care-plan-activity-outcome,ValueSet/procedure-category,ValueSet/condition-code,ValueSet/condition-stage-type,ValueSet/immunization-status-reason,ValueSet/procedure-not-performed-reason,ValueSet/care-plan-category,ValueSet/us-core-procedure-code,ValueSet/observation-methods,ValueSet/questionnaire-answers,ValueSet/servicerequest-orderdetail,ValueSet/administration-method-codes,ValueSet/condition-severity</t>
-        </is>
-      </c>
-      <c r="I52" t="inlineStr"/>
+          <t>LOINC provides a set of universal names and ID codes for identifying laboratory and clinical test results.1,2 LOINC facilitates the exchange and pooling of results, such as blood hemoglobin, serum potassium, or vital signs, for clinical care, outcomes management, and research. LOINC's universal identifiers (names and codes) can be used in the context of order and observation exchanges between information systems that use syntax standards such as HL73, CEN TC251, ISO TC215, ASTM4, and DICOM. Specifically, the identifier can be used as the coded value for an observation in any other standard that uses the observation/observation value paradigm, whether messages, documents, application programming interface (API), etc. For example, LOINC codes are used widely in the OBX segment Observation Identifier field (OBX-3) of an ORU HL7 (HL7 version 2.x or ASTM 1238-9410) message that may be sent between a Clinical Laboratory Information Management Systems (LIMS) and Electronic Health Record Systems (EHR).5, 6 In this way, LOINC codes provide universal identifiers that allow the exchange of clinical data between heterogeneous computing environments.</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>ValueSet/us-core-diagnosticreport-category,ValueSet/c80-doc-typecodes,ValueSet/us-core-documentreference-type,ValueSet/2.16.840.1.113883.3.88.12.80.62,ValueSet/document-classcodes,ValueSet/2.16.840.1.113762.1.4.1267.13,ValueSet/us-core-clinical-note-type,ValueSet/us-core-goal-description,ValueSet/us-core-laboratory-test-codes,ValueSet/care-team-category,ValueSet/us-core-diagnosticreport-report-and-note-codes,ValueSet/2.16.840.1.113883.11.20.9.69.4,ValueSet/us-core-procedure-code,ValueSet/observation-codes</t>
+        </is>
+      </c>
       <c r="J52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/PHOccupationalDataForHealthODH</t>
+          <t>http://snomed.info/sct</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>2.0.1</t>
+          <t>null</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2730,27 +2730,27 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>2.16.840.1.114222.4.5.327</t>
+          <t>2.16.840.1.113883.6.96</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>PHOccupationalDataForHealthODH</t>
+          <t>SNOMED_CT</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Occupational Data for Health (ODH)</t>
+          <t>SNOMED CT (all versions)</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>The concepts representing the values supporting Occupational Data for Health, including Job Supervisory Level or Pay Grade (ODH) code system consists of data elements that describe a person's work information, structured to facilitate individual, population, and public health use; not intended to support billing.).</t>
+          <t>SNOMED CT is the most comprehensive and precise clinical health terminology product in the world, owned and distributed around the world by The International Health Terminology Standards Development Organisation (IHTSDO).</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>ValueSet/2.16.840.1.114222.4.11.7900,ValueSet/2.16.840.1.114222.4.11.7901</t>
+          <t>ValueSet/servicerequest-category,ValueSet/specimen-container-type,ValueSet/2.16.840.1.113762.1.4.1099.54,ValueSet/procedure-followup,ValueSet/us-core-goal-description,ValueSet/us-core-condition-code-current,ValueSet/specimen-collection-method,ValueSet/medication-form-codes,ValueSet/body-site,ValueSet/manifestation-or-symptom,ValueSet/goal-start-event,ValueSet/procedure-code,ValueSet/medication-as-needed-reason,ValueSet/2.16.840.1.113762.1.4.1166.22,ValueSet/c80-facilitycodes,ValueSet/immunization-reason,ValueSet/2.16.840.1.113762.1.4.1267.3,ValueSet/substance-code,ValueSet/care-plan-category,ValueSet/us-core-procedure-code,ValueSet/observation-methods,ValueSet/questionnaire-answers,ValueSet/servicerequest-orderdetail,ValueSet/clinical-findings,ValueSet/condition-stage,ValueSet/encounter-reason,ValueSet/immunization-target-disease,ValueSet/additional-instruction-codes,ValueSet/participant-role,ValueSet/approach-site-codes,ValueSet/device-action,ValueSet/us-core-condition-code,ValueSet/medication-codes,ValueSet/device-kind,ValueSet/performer-role,ValueSet/us-core-servicerequest-category,ValueSet/referencerange-appliesto,ValueSet/c80-practice-codes,ValueSet/route-codes,ValueSet/care-plan-activity-outcome,ValueSet/procedure-outcome,ValueSet/procedure-category,ValueSet/2.16.840.1.113762.1.4.1021.121,ValueSet/condition-code,ValueSet/2.16.840.1.113762.1.4.1267.26,ValueSet/condition-stage-type,ValueSet/immunization-status-reason,ValueSet/procedure-not-performed-reason,ValueSet/administration-method-codes,ValueSet/condition-severity</t>
         </is>
       </c>
       <c r="I53" t="inlineStr"/>
@@ -2759,12 +2759,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/admit-source</t>
+          <t>http://terminology.hl7.org/CodeSystem/PHOccupationalDataForHealthODH</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>1.0.1</t>
+          <t>2.0.1</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2774,27 +2774,27 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1092</t>
+          <t>2.16.840.1.114222.4.5.327</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>AdmitSource</t>
+          <t>PHOccupationalDataForHealthODH</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Admit source</t>
+          <t>Occupational Data for Health (ODH)</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>This value set defines a set of codes that can be used to indicate from where the patient came in.</t>
+          <t>The concepts representing the values supporting Occupational Data for Health, including Job Supervisory Level or Pay Grade (ODH) code system consists of data elements that describe a person's work information, structured to facilitate individual, population, and public health use; not intended to support billing.).</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>ValueSet/encounter-admit-source</t>
+          <t>ValueSet/2.16.840.1.114222.4.11.7900,ValueSet/2.16.840.1.114222.4.11.7901</t>
         </is>
       </c>
       <c r="I54" t="inlineStr"/>
@@ -2803,42 +2803,42 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/allergyintolerance-clinical</t>
+          <t>http://terminology.hl7.org/CodeSystem/admit-source</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>1.0.1</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1373</t>
+          <t>2.16.840.1.113883.4.642.1.1092</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>AllergyIntoleranceClinicalStatusCodes</t>
+          <t>AdmitSource</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>AllergyIntolerance Clinical Status Codes</t>
+          <t>Admit source</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Preferred value set for AllergyIntolerance Clinical Status.</t>
+          <t>This value set defines a set of codes that can be used to indicate from where the patient came in.</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>ValueSet/allergyintolerance-clinical</t>
+          <t>ValueSet/encounter-admit-source</t>
         </is>
       </c>
       <c r="I55" t="inlineStr"/>
@@ -2847,42 +2847,42 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/allergyintolerance-verification</t>
+          <t>http://terminology.hl7.org/CodeSystem/allergyintolerance-clinical</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>1.0.1</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1371</t>
+          <t>2.16.840.1.113883.4.642.1.1373</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>AllergyIntoleranceVerificationStatus</t>
+          <t>AllergyIntoleranceClinicalStatusCodes</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>AllergyIntolerance Verification Status</t>
+          <t>AllergyIntolerance Clinical Status Codes</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>The verification status to support or decline the clinical status of the allergy or intolerance.</t>
+          <t>Preferred value set for AllergyIntolerance Clinical Status.</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>ValueSet/allergyintolerance-verification</t>
+          <t>ValueSet/allergyintolerance-clinical</t>
         </is>
       </c>
       <c r="I56" t="inlineStr"/>
@@ -2891,42 +2891,42 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/common-tags</t>
+          <t>http://terminology.hl7.org/CodeSystem/allergyintolerance-verification</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>1.0.1</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1067</t>
+          <t>2.16.840.1.113883.4.642.1.1371</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>CommonTags</t>
+          <t>AllergyIntoleranceVerificationStatus</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Common Tags</t>
+          <t>AllergyIntolerance Verification Status</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>Common Tag Codes defined by FHIR project</t>
+          <t>The verification status to support or decline the clinical status of the allergy or intolerance.</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>ValueSet/common-tags</t>
+          <t>ValueSet/allergyintolerance-verification</t>
         </is>
       </c>
       <c r="I57" t="inlineStr"/>
@@ -2935,42 +2935,42 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/condition-category</t>
+          <t>http://terminology.hl7.org/CodeSystem/common-tags</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>1.0.1</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1073</t>
+          <t>2.16.840.1.113883.4.642.1.1067</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>ConditionCategoryCodes</t>
+          <t>CommonTags</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Condition Category Codes</t>
+          <t>Common Tags</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Preferred value set for Condition Categories.</t>
+          <t>Common Tag Codes defined by FHIR project</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>ValueSet/condition-category,ValueSet/us-core-problem-or-health-concern</t>
+          <t>ValueSet/common-tags</t>
         </is>
       </c>
       <c r="I58" t="inlineStr"/>
@@ -2979,42 +2979,42 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/condition-clinical</t>
+          <t>http://terminology.hl7.org/CodeSystem/condition-category</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>3.0.0</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1074</t>
+          <t>2.16.840.1.113883.4.642.1.1073</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>ConditionClinicalStatusCodes</t>
+          <t>ConditionCategoryCodes</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Condition Clinical Status Codes</t>
+          <t>Condition Category Codes</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Preferred value set for Condition Clinical Status.</t>
+          <t>Preferred value set for Condition Categories.</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>ValueSet/condition-clinical</t>
+          <t>ValueSet/condition-category,ValueSet/us-core-problem-or-health-concern</t>
         </is>
       </c>
       <c r="I59" t="inlineStr"/>
@@ -3023,12 +3023,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/condition-ver-status</t>
+          <t>http://terminology.hl7.org/CodeSystem/condition-clinical</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>2.0.1</t>
+          <t>3.0.0</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -3038,27 +3038,27 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1075</t>
+          <t>2.16.840.1.113883.4.642.1.1074</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>ConditionVerificationStatus</t>
+          <t>ConditionClinicalStatusCodes</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>ConditionVerificationStatus</t>
+          <t>Condition Clinical Status Codes</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>The verification status to support or decline the clinical status of the condition or diagnosis.</t>
+          <t>Preferred value set for Condition Clinical Status.</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>ValueSet/condition-ver-status</t>
+          <t>ValueSet/condition-clinical</t>
         </is>
       </c>
       <c r="I60" t="inlineStr"/>
@@ -3067,12 +3067,12 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/contactentity-type</t>
+          <t>http://terminology.hl7.org/CodeSystem/condition-ver-status</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>1.0.0</t>
+          <t>2.0.0</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -3082,27 +3082,27 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1129</t>
+          <t>2.16.840.1.113883.4.642.1.1075</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>ContactEntityType</t>
+          <t>ConditionVerificationStatus</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Contact entity type</t>
+          <t>ConditionVerificationStatus</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>This example value set defines a set of codes that can be used to indicate the purpose for which you would contact a contact party.</t>
+          <t>The verification status to support or decline the clinical status of the condition or diagnosis.</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>ValueSet/contactentity-type</t>
+          <t>ValueSet/condition-ver-status</t>
         </is>
       </c>
       <c r="I61" t="inlineStr"/>
@@ -3111,42 +3111,42 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/contractsignertypecodes</t>
+          <t>http://terminology.hl7.org/CodeSystem/contactentity-type</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>1.0.1</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1201</t>
+          <t>2.16.840.1.113883.4.642.1.1129</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>ContractSignerTypeCodes</t>
+          <t>ContactEntityType</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Contract Signer Type Codes</t>
+          <t>Contact entity type</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>This value set includes sample Contract Signer Type codes.</t>
+          <t>This example value set defines a set of codes that can be used to indicate the purpose for which you would contact a contact party.</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>ValueSet/security-role-type</t>
+          <t>ValueSet/contactentity-type</t>
         </is>
       </c>
       <c r="I62" t="inlineStr"/>
@@ -3155,42 +3155,42 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/coverage-class</t>
+          <t>http://terminology.hl7.org/CodeSystem/contractsignertypecodes</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>1.0.1</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1147</t>
+          <t>2.16.840.1.113883.4.642.1.1201</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>CoverageClassCodes</t>
+          <t>ContractSignerTypeCodes</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Coverage Class Codes</t>
+          <t>Contract Signer Type Codes</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>This value set includes Coverage Class codes.</t>
+          <t>This value set includes sample Contract Signer Type codes.</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>ValueSet/coverage-class</t>
+          <t>ValueSet/security-role-type</t>
         </is>
       </c>
       <c r="I63" t="inlineStr"/>
@@ -3199,42 +3199,42 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/coverage-copay-type</t>
+          <t>http://terminology.hl7.org/CodeSystem/coverage-class</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>1.0.1</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1149</t>
+          <t>2.16.840.1.113883.4.642.1.1147</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>CoverageCopayTypeCodes</t>
+          <t>CoverageClassCodes</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Coverage Copay Type Codes</t>
+          <t>Coverage Class Codes</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>This value set includes sample Coverage Copayment Type codes.</t>
+          <t>This value set includes Coverage Class codes.</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>ValueSet/coverage-copay-type</t>
+          <t>ValueSet/coverage-class</t>
         </is>
       </c>
       <c r="I64" t="inlineStr"/>
@@ -3243,7 +3243,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/data-absent-reason</t>
+          <t>http://terminology.hl7.org/CodeSystem/coverage-copay-type</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -3253,32 +3253,32 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.4.1048</t>
+          <t>2.16.840.1.113883.4.642.1.1149</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>DataAbsentReason</t>
+          <t>CoverageCopayTypeCodes</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>DataAbsentReason</t>
+          <t>Coverage Copay Type Codes</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>Used to specify why the normally expected content of the data element is missing.</t>
+          <t>This value set includes sample Coverage Copayment Type codes.</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>ValueSet/data-absent-reason</t>
+          <t>ValueSet/coverage-copay-type</t>
         </is>
       </c>
       <c r="I65" t="inlineStr"/>
@@ -3287,7 +3287,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/device-status-reason</t>
+          <t>http://terminology.hl7.org/CodeSystem/data-absent-reason</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -3297,32 +3297,32 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>draft</t>
+          <t>active</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1082</t>
+          <t>2.16.840.1.113883.4.642.4.1048</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>FHIRDeviceStatusReason</t>
+          <t>DataAbsentReason</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>FHIRDeviceStatusReason</t>
+          <t>DataAbsentReason</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>The availability status reason of the device.</t>
+          <t>Used to specify why the normally expected content of the data element is missing.</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>ValueSet/device-status-reason</t>
+          <t>ValueSet/data-absent-reason</t>
         </is>
       </c>
       <c r="I66" t="inlineStr"/>
@@ -3331,42 +3331,42 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/diagnosis-role</t>
+          <t>http://terminology.hl7.org/CodeSystem/device-status-reason</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>1.1.1</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1054</t>
+          <t>2.16.840.1.113883.4.642.1.1082</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>DiagnosisRole</t>
+          <t>FHIRDeviceStatusReason</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Diagnosis Role</t>
+          <t>FHIRDeviceStatusReason</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>This value set defines a set of codes that can be used to express the role of a diagnosis on the Encounter or EpisodeOfCare record.</t>
+          <t>The availability status reason of the device.</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>ValueSet/diagnosis-role</t>
+          <t>ValueSet/device-status-reason</t>
         </is>
       </c>
       <c r="I67" t="inlineStr"/>
@@ -3375,42 +3375,42 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/diet</t>
+          <t>http://terminology.hl7.org/CodeSystem/diagnosis-role</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>1.0.1</t>
+          <t>1.1.0</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1091</t>
+          <t>2.16.840.1.113883.4.642.1.1054</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Diet</t>
+          <t>DiagnosisRole</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Diet</t>
+          <t>Diagnosis Role</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>This value set defines a set of codes that can be used to indicate dietary preferences or restrictions a patient may have.</t>
+          <t>This value set defines a set of codes that can be used to express the role of a diagnosis on the Encounter or EpisodeOfCare record.</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>ValueSet/encounter-diet</t>
+          <t>ValueSet/diagnosis-role</t>
         </is>
       </c>
       <c r="I68" t="inlineStr"/>
@@ -3419,7 +3419,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/dose-rate-type</t>
+          <t>http://terminology.hl7.org/CodeSystem/diet</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -3434,27 +3434,27 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1069</t>
+          <t>2.16.840.1.113883.4.642.1.1091</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>DoseAndRateType</t>
+          <t>Diet</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>DoseAndRateType</t>
+          <t>Diet</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>The kind of dose or rate specified.</t>
+          <t>This value set defines a set of codes that can be used to indicate dietary preferences or restrictions a patient may have.</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>ValueSet/dose-rate-type</t>
+          <t>ValueSet/encounter-diet</t>
         </is>
       </c>
       <c r="I69" t="inlineStr"/>
@@ -3463,42 +3463,42 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/encounter-special-arrangements</t>
+          <t>http://terminology.hl7.org/CodeSystem/dose-rate-type</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>1.0.1</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1090</t>
+          <t>2.16.840.1.113883.4.642.1.1069</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>SpecialArrangements</t>
+          <t>DoseAndRateType</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>Special arrangements</t>
+          <t>DoseAndRateType</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>This value set defines a set of codes that can be used to indicate the kinds of special arrangements in place for a patients visit.</t>
+          <t>The kind of dose or rate specified.</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>ValueSet/encounter-special-arrangements</t>
+          <t>ValueSet/dose-rate-type</t>
         </is>
       </c>
       <c r="I70" t="inlineStr"/>
@@ -3507,42 +3507,42 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/ex-coverage-financial-exception</t>
+          <t>http://terminology.hl7.org/CodeSystem/encounter-special-arrangements</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>1.0.1</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1329</t>
+          <t>2.16.840.1.113883.4.642.1.1090</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>ExampleCoverageFinancialExceptionCodes</t>
+          <t>SpecialArrangements</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>Example Coverage Financial Exception Codes</t>
+          <t>Special arrangements</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>This value set includes Example Coverage Financial Exception Codes.</t>
+          <t>This value set defines a set of codes that can be used to indicate the kinds of special arrangements in place for a patients visit.</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>ValueSet/coverage-financial-exception</t>
+          <t>ValueSet/encounter-special-arrangements</t>
         </is>
       </c>
       <c r="I71" t="inlineStr"/>
@@ -3551,38 +3551,42 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/extra-security-role-type</t>
+          <t>http://terminology.hl7.org/CodeSystem/ex-coverage-financial-exception</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>1.0.1</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>active</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr"/>
+          <t>draft</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>2.16.840.1.113883.4.642.1.1329</t>
+        </is>
+      </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>SecurityRoleType</t>
+          <t>ExampleCoverageFinancialExceptionCodes</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Security Role Type</t>
+          <t>Example Coverage Financial Exception Codes</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>This CodeSystem contains Additional FHIR-defined Security Role types not defined elsewhere</t>
+          <t>This value set includes Example Coverage Financial Exception Codes.</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>ValueSet/security-role-type</t>
+          <t>ValueSet/coverage-financial-exception</t>
         </is>
       </c>
       <c r="I72" t="inlineStr"/>
@@ -3591,42 +3595,38 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/goal-achievement</t>
+          <t>http://terminology.hl7.org/CodeSystem/extra-security-role-type</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>1.0.1</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>active</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>2.16.840.1.113883.4.642.1.1375</t>
-        </is>
-      </c>
+          <t>draft</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr"/>
       <c r="E73" t="inlineStr">
         <is>
-          <t>GoalAchievementStatus</t>
+          <t>SecurityRoleType</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Goal achievement status</t>
+          <t>Security Role Type</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>Describes the progression, or lack thereof, towards the goal against the target.</t>
+          <t>This CodeSystem contains Additional FHIR-defined Security Role types not defined elsewhere</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>ValueSet/goal-achievement</t>
+          <t>ValueSet/security-role-type</t>
         </is>
       </c>
       <c r="I73" t="inlineStr"/>
@@ -3635,42 +3635,42 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/goal-category</t>
+          <t>http://terminology.hl7.org/CodeSystem/goal-achievement</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>1.0.1</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1097</t>
+          <t>2.16.840.1.113883.4.642.1.1375</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>GoalCategory</t>
+          <t>GoalAchievementStatus</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Goal category</t>
+          <t>Goal achievement status</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Example codes for grouping goals to use for filtering or presentation.</t>
+          <t>Describes the progression, or lack thereof, towards the goal against the target.</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>ValueSet/goal-category</t>
+          <t>ValueSet/goal-achievement</t>
         </is>
       </c>
       <c r="I74" t="inlineStr"/>
@@ -3679,12 +3679,12 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/goal-priority</t>
+          <t>http://terminology.hl7.org/CodeSystem/goal-category</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>1.0.1</t>
+          <t>2.0.0</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -3694,27 +3694,27 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1096</t>
+          <t>2.16.840.1.113883.4.642.1.1097</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>GoalPriority</t>
+          <t>GoalCategory</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Goal priority</t>
+          <t>Goal category</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Indicates the level of importance associated with reaching or sustaining a goal.</t>
+          <t>Codes for grouping goals to use for filtering or presentation.</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>ValueSet/goal-priority</t>
+          <t>ValueSet/goal-category</t>
         </is>
       </c>
       <c r="I75" t="inlineStr"/>
@@ -3723,42 +3723,42 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/icd9cm</t>
+          <t>http://terminology.hl7.org/CodeSystem/goal-priority</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>2.0.1</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>retired</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.6.2</t>
+          <t>2.16.840.1.113883.4.642.1.1096</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Icd9cm</t>
+          <t>GoalPriority</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>ICD-9CM</t>
+          <t>Goal priority</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>International Classification of Diseases revision 9, with Clinical Modifications (ICD 9 CM)</t>
+          <t>Indicates the level of importance associated with reaching or sustaining a goal.</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>ValueSet/us-core-condition-code</t>
+          <t>ValueSet/goal-priority</t>
         </is>
       </c>
       <c r="I76" t="inlineStr"/>
@@ -3767,42 +3767,42 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/immunization-funding-source</t>
+          <t>http://terminology.hl7.org/CodeSystem/icd9cm</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>1.0.1</t>
+          <t>2.0.1</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>retired</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1100</t>
+          <t>2.16.840.1.113883.6.2</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>ImmunizationFundingSource</t>
+          <t>Icd9cm</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Immunization Funding Source</t>
+          <t>ICD-9CM</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>The value set to instantiate this attribute should be drawn from a terminologically robust code system that consists of or contains concepts to support describing the source of the vaccine administered. This value set is provided as a suggestive example.</t>
+          <t>International Classification of Diseases revision 9, with Clinical Modifications (ICD 9 CM)</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>ValueSet/immunization-funding-source</t>
+          <t>ValueSet/us-core-condition-code</t>
         </is>
       </c>
       <c r="I77" t="inlineStr"/>
@@ -3811,42 +3811,42 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/immunization-origin</t>
+          <t>http://terminology.hl7.org/CodeSystem/immunization-funding-source</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>1.0.1</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1101</t>
+          <t>2.16.840.1.113883.4.642.1.1100</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>ImmunizationOriginCodes</t>
+          <t>ImmunizationFundingSource</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Immunization Origin Codes</t>
+          <t>Immunization Funding Source</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>The value set to instantiate this attribute should be drawn from a terminologically robust code system that consists of or contains concepts to support describing the source of the data when the report of the immunization event is not based on information from the person, entity or organization who administered the vaccine. This value set is provided as a suggestive example.</t>
+          <t>The value set to instantiate this attribute should be drawn from a terminologically robust code system that consists of or contains concepts to support describing the source of the vaccine administered. This value set is provided as a suggestive example.</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>ValueSet/immunization-origin</t>
+          <t>ValueSet/immunization-funding-source</t>
         </is>
       </c>
       <c r="I78" t="inlineStr"/>
@@ -3855,42 +3855,42 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/immunization-program-eligibility</t>
+          <t>http://terminology.hl7.org/CodeSystem/immunization-origin</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>1.0.1</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1099</t>
+          <t>2.16.840.1.113883.4.642.1.1101</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>ImmunizationProgramEligibility</t>
+          <t>ImmunizationOriginCodes</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Immunization Program Eligibility</t>
+          <t>Immunization Origin Codes</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>The value set to instantiate this attribute should be drawn from a terminologically robust code system that consists of or contains concepts to support describing the patient's eligibility for a vaccination program. This value set is provided as a suggestive example.</t>
+          <t>The value set to instantiate this attribute should be drawn from a terminologically robust code system that consists of or contains concepts to support describing the source of the data when the report of the immunization event is not based on information from the person, entity or organization who administered the vaccine. This value set is provided as a suggestive example.</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>ValueSet/immunization-program-eligibility</t>
+          <t>ValueSet/immunization-origin</t>
         </is>
       </c>
       <c r="I79" t="inlineStr"/>
@@ -3899,42 +3899,42 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/immunization-subpotent-reason</t>
+          <t>http://terminology.hl7.org/CodeSystem/immunization-program-eligibility</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>1.0.1</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1098</t>
+          <t>2.16.840.1.113883.4.642.1.1099</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>ImmunizationSubpotentReason</t>
+          <t>ImmunizationProgramEligibility</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Immunization Subpotent Reason</t>
+          <t>Immunization Program Eligibility</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>The value set to instantiate this attribute should be drawn from a terminologically robust code system that consists of or contains concepts to support describing the reason why a dose is considered to be subpotent. This value set is provided as a suggestive example.</t>
+          <t>The value set to instantiate this attribute should be drawn from a terminologically robust code system that consists of or contains concepts to support describing the patient's eligibility for a vaccination program. This value set is provided as a suggestive example.</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>ValueSet/immunization-subpotent-reason</t>
+          <t>ValueSet/immunization-program-eligibility</t>
         </is>
       </c>
       <c r="I80" t="inlineStr"/>
@@ -3943,42 +3943,42 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/location-physical-type</t>
+          <t>http://terminology.hl7.org/CodeSystem/immunization-subpotent-reason</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>2.0.1</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1108</t>
+          <t>2.16.840.1.113883.4.642.1.1098</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>LocationType</t>
+          <t>ImmunizationSubpotentReason</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Location type</t>
+          <t>Immunization Subpotent Reason</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>This example value set defines a set of codes that can be used to indicate the physical form of the Location.  This includes several 'non physical' codes which are still considered a location.</t>
+          <t>The value set to instantiate this attribute should be drawn from a terminologically robust code system that consists of or contains concepts to support describing the reason why a dose is considered to be subpotent. This value set is provided as a suggestive example.</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>ValueSet/location-physical-type</t>
+          <t>ValueSet/immunization-subpotent-reason</t>
         </is>
       </c>
       <c r="I81" t="inlineStr"/>
@@ -3987,42 +3987,42 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/medicationdispense-performer-function</t>
+          <t>http://terminology.hl7.org/CodeSystem/location-physical-type</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>1.0.1</t>
+          <t>2.0.0</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1319</t>
+          <t>2.16.840.1.113883.4.642.1.1108</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>MedicationDispensePerformerFunctionCodes</t>
+          <t>LocationType</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>MedicationDispense Performer Function Codes</t>
+          <t>Location type</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>MedicationDispense Performer Function Codes</t>
+          <t>This example value set defines a set of codes that can be used to indicate the physical form of the Location.  This includes several 'non physical' codes which are still considered a location.</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>ValueSet/medicationdispense-performer-function</t>
+          <t>ValueSet/location-physical-type</t>
         </is>
       </c>
       <c r="I82" t="inlineStr"/>
@@ -4031,12 +4031,12 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/medicationdispense-status</t>
+          <t>http://terminology.hl7.org/CodeSystem/medicationdispense-performer-function</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>4.0.1</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -4046,27 +4046,27 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.4.1313</t>
+          <t>2.16.840.1.113883.4.642.1.1319</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>MedicationDispense Status Codes</t>
+          <t>MedicationDispensePerformerFunctionCodes</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Medication dispense  status  codes</t>
+          <t>MedicationDispense Performer Function Codes</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>MedicationDispense Status Codes</t>
+          <t>MedicationDispense Performer Function Codes</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>ValueSet/medicationdispense-status</t>
+          <t>ValueSet/medicationdispense-performer-function</t>
         </is>
       </c>
       <c r="I83" t="inlineStr"/>
@@ -4075,12 +4075,12 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/medicationrequest-category</t>
+          <t>http://terminology.hl7.org/CodeSystem/medicationdispense-status</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>1.0.0</t>
+          <t>4.0.1</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -4090,27 +4090,27 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1323</t>
+          <t>2.16.840.1.113883.4.642.4.1313</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>MedicationRequestCategoryCodes</t>
+          <t>MedicationDispense Status Codes</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>MedicationRequest Category Codes</t>
+          <t>Medication dispense  status  codes</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>MedicationRequest Category Codes</t>
+          <t>MedicationDispense Status Codes</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>ValueSet/medicationrequest-category</t>
+          <t>ValueSet/medicationdispense-status</t>
         </is>
       </c>
       <c r="I84" t="inlineStr"/>
@@ -4119,42 +4119,42 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/medicationrequest-course-of-therapy</t>
+          <t>http://terminology.hl7.org/CodeSystem/medicationrequest-category</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>1.0.1</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1327</t>
+          <t>2.16.840.1.113883.4.642.1.1323</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>MedicationRequestCourseOfTherapyCodes</t>
+          <t>MedicationRequestCategoryCodes</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>MedicationRequest Course of Therapy Codes</t>
+          <t>MedicationRequest Category Codes</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>MedicationRequest Course of Therapy Codes</t>
+          <t>MedicationRequest Category Codes</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>ValueSet/medicationrequest-course-of-therapy</t>
+          <t>ValueSet/medicationrequest-category</t>
         </is>
       </c>
       <c r="I85" t="inlineStr"/>
@@ -4163,42 +4163,42 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/medicationrequest-status-reason</t>
+          <t>http://terminology.hl7.org/CodeSystem/medicationrequest-course-of-therapy</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>1.0.1</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1325</t>
+          <t>2.16.840.1.113883.4.642.1.1327</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>MedicationRequestStatusReasonCodes</t>
+          <t>MedicationRequestCourseOfTherapyCodes</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>MedicationRequest Status Reason Codes</t>
+          <t>MedicationRequest Course of Therapy Codes</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>MedicationRequest Status Reason Codes</t>
+          <t>MedicationRequest Course of Therapy Codes</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>ValueSet/medicationrequest-status-reason</t>
+          <t>ValueSet/medicationrequest-course-of-therapy</t>
         </is>
       </c>
       <c r="I86" t="inlineStr"/>
@@ -4207,60 +4207,56 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/nubc-UB92</t>
+          <t>http://terminology.hl7.org/CodeSystem/medicationrequest-status-reason</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>2.0.1</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.6.21</t>
+          <t>2.16.840.1.113883.4.642.1.1325</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>NubcUB92</t>
+          <t>MedicationRequestStatusReasonCodes</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>National Uniform Billing Council</t>
+          <t>MedicationRequest Status Reason Codes</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t xml:space="preserve"> UB 92</t>
+          <t>MedicationRequest Status Reason Codes</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>National Uniform Billing Council, UB 92</t>
-        </is>
-      </c>
-      <c r="I87" t="inlineStr">
-        <is>
-          <t>ValueSet/v3-USEncounterDischargeDisposition</t>
-        </is>
-      </c>
+          <t>ValueSet/medicationrequest-status-reason</t>
+        </is>
+      </c>
+      <c r="I87" t="inlineStr"/>
       <c r="J87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/observation-category</t>
+          <t>http://terminology.hl7.org/CodeSystem/nubc-UB92</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>1.0.1</t>
+          <t>2.0.1</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -4270,71 +4266,75 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1125</t>
+          <t>2.16.840.1.113883.6.21</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>ObservationCategoryCodes</t>
+          <t>NubcUB92</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>Observation Category Codes</t>
+          <t>National Uniform Billing Council</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>Observation Category codes.</t>
+          <t xml:space="preserve"> UB 92</t>
         </is>
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>ValueSet/us-core-screening-assessment-observation-category,ValueSet/us-core-simple-observation-category,ValueSet/us-core-clinical-result-observation-category,ValueSet/observation-category,ValueSet/us-core-screening-assessment-observation-maximum-category</t>
-        </is>
-      </c>
-      <c r="I88" t="inlineStr"/>
+          <t>National Uniform Billing Council, UB 92</t>
+        </is>
+      </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>ValueSet/v3-USEncounterDischargeDisposition</t>
+        </is>
+      </c>
       <c r="J88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/organization-type</t>
+          <t>http://terminology.hl7.org/CodeSystem/observation-category</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>2.0.1</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1128</t>
+          <t>2.16.840.1.113883.4.642.1.1125</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>OrganizationType</t>
+          <t>ObservationCategoryCodes</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>Organization type</t>
+          <t>Observation Category Codes</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>This example value set defines a set of codes that can be used to indicate a type of organization.</t>
+          <t>Observation Category codes.</t>
         </is>
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>ValueSet/organization-type</t>
+          <t>ValueSet/us-core-screening-assessment-observation-category,ValueSet/us-core-simple-observation-category,ValueSet/us-core-clinical-result-observation-category,ValueSet/observation-category,ValueSet/us-core-screening-assessment-observation-maximum-category</t>
         </is>
       </c>
       <c r="I89" t="inlineStr"/>
@@ -4343,42 +4343,42 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/participant-type</t>
+          <t>http://terminology.hl7.org/CodeSystem/organization-type</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>1.0.1</t>
+          <t>2.0.0</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1089</t>
+          <t>2.16.840.1.113883.4.642.1.1128</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>ParticipantType</t>
+          <t>OrganizationType</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Participant type</t>
+          <t>Organization type</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>This value set defines a set of codes that can be used to indicate how an individual participates in an encounter.</t>
+          <t>This example value set defines a set of codes that can be used to indicate a type of organization.</t>
         </is>
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>ValueSet/encounter-participant-type</t>
+          <t>ValueSet/organization-type</t>
         </is>
       </c>
       <c r="I90" t="inlineStr"/>
@@ -4387,42 +4387,42 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/provenance-participant-type</t>
+          <t>http://terminology.hl7.org/CodeSystem/participant-type</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>1.1.0</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1131</t>
+          <t>2.16.840.1.113883.4.642.1.1089</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>ProvenanceParticipantType</t>
+          <t>ParticipantType</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Provenance participant type</t>
+          <t>Participant type</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>These codes define the type of participation by an agent in a provenance activity. An agent is something that bears the responsibility identified by the type of participation in the activity taking place, for the existence of an entity, or for another agent's activity. An Agent may be An agent, device, system, organization, group, care-team, or other identifiable thing.</t>
+          <t>This value set defines a set of codes that can be used to indicate how an individual participates in an encounter.</t>
         </is>
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>ValueSet/provenance-agent-type</t>
+          <t>ValueSet/encounter-participant-type</t>
         </is>
       </c>
       <c r="I91" t="inlineStr"/>
@@ -4431,12 +4431,12 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/referencerange-meaning</t>
+          <t>http://terminology.hl7.org/CodeSystem/provenance-participant-type</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>1.0.1</t>
+          <t>1.1.0</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -4446,27 +4446,27 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1124</t>
+          <t>2.16.840.1.113883.4.642.1.1131</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>ObservationReferenceRangeMeaningCodes</t>
+          <t>ProvenanceParticipantType</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>Observation Reference Range Meaning Codes</t>
+          <t>Provenance participant type</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>This value set defines a set of codes that can be used to indicate the meaning/use of a reference range for a particular target population.</t>
+          <t>These codes define the type of participation by an agent in a provenance activity. An agent is something that bears the responsibility identified by the type of participation in the activity taking place, for the existence of an entity, or for another agent's activity. An Agent may be An agent, device, system, organization, group, care-team, or other identifiable thing.</t>
         </is>
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>ValueSet/referencerange-meaning</t>
+          <t>ValueSet/us-core-provenance-participant-type</t>
         </is>
       </c>
       <c r="I92" t="inlineStr"/>
@@ -4475,42 +4475,42 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/service-type</t>
+          <t>http://terminology.hl7.org/CodeSystem/referencerange-meaning</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>1.1.1</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1145</t>
+          <t>2.16.840.1.113883.4.642.1.1124</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>ServiceType</t>
+          <t>ObservationReferenceRangeMeaningCodes</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Service type</t>
+          <t>Observation Reference Range Meaning Codes</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>This value set defines an example set of codes of service-types.</t>
+          <t>This value set defines a set of codes that can be used to indicate the meaning/use of a reference range for a particular target population.</t>
         </is>
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>ValueSet/service-type</t>
+          <t>ValueSet/referencerange-meaning</t>
         </is>
       </c>
       <c r="I93" t="inlineStr"/>
@@ -4519,42 +4519,42 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/subscriber-relationship</t>
+          <t>http://terminology.hl7.org/CodeSystem/service-type</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>1.0.1</t>
+          <t>1.1.0</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1386</t>
+          <t>2.16.840.1.113883.4.642.1.1145</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>SubscriberRelationshipCodes</t>
+          <t>ServiceType</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>SubscriberPolicyholder Relationship Codes</t>
+          <t>Service type</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>This value set includes codes for the relationship between the Subscriber and the Beneficiary (insured/covered party/patient).</t>
+          <t>This value set defines an example set of codes of service-types.</t>
         </is>
       </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>ValueSet/subscriber-relationship</t>
+          <t>ValueSet/service-type</t>
         </is>
       </c>
       <c r="I94" t="inlineStr"/>
@@ -4563,42 +4563,42 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v2-0074</t>
+          <t>http://terminology.hl7.org/CodeSystem/subscriber-relationship</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>2.0.0</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.18.29</t>
+          <t>2.16.840.1.113883.4.642.1.1386</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>DiagnosticServiceSectionId</t>
+          <t>SubscriberRelationshipCodes</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>diagnosticServiceSectionId</t>
+          <t>SubscriberPolicyholder Relationship Codes</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>HL7-defined code system of concepts which specify a section of a diagnostic service where the observation may be performed.  Used in HL7 Version 2.x messaging in the OBR and OM4 segments.</t>
+          <t>This value set includes codes for the relationship between the Subscriber and the Beneficiary (insured/covered party/patient).</t>
         </is>
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>ValueSet/diagnostic-service-sections</t>
+          <t>ValueSet/subscriber-relationship</t>
         </is>
       </c>
       <c r="I95" t="inlineStr"/>
@@ -4607,7 +4607,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v2-0092</t>
+          <t>http://terminology.hl7.org/CodeSystem/v2-0074</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -4622,27 +4622,27 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.18.36</t>
+          <t>2.16.840.1.113883.18.29</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>ReAdmissionIndicator</t>
+          <t>DiagnosticServiceSectionId</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>re-admissionIndicator</t>
+          <t>diagnosticServiceSectionId</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>Code system of concepts which are used to specify that a patient is being re admitted to a healthcare facilityin from which they were discharged, and indicates the circumstances around such re-admission.  Used in HL7 Version 2.x messagine in the PV1 segment.</t>
+          <t>HL7-defined code system of concepts which specify a section of a diagnostic service where the observation may be performed.  Used in HL7 Version 2.x messaging in the OBR and OM4 segments.</t>
         </is>
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>ValueSet/v2-0092</t>
+          <t>ValueSet/diagnostic-service-sections</t>
         </is>
       </c>
       <c r="I96" t="inlineStr"/>
@@ -4651,7 +4651,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v2-0116</t>
+          <t>http://terminology.hl7.org/CodeSystem/v2-0092</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -4666,27 +4666,27 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.18.47</t>
+          <t>2.16.840.1.113883.18.36</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>BedStatus</t>
+          <t>ReAdmissionIndicator</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>bedStatus</t>
+          <t>re-admissionIndicator</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>Code system of concepts which specify the state of a bed in an inpatient setting, and is used to determine if a patient may be assigned to it or not.  Used in HL7 Version 2.x messaging in the DLD and PV1 segments.</t>
+          <t>Code system of concepts which are used to specify that a patient is being re admitted to a healthcare facilityin from which they were discharged, and indicates the circumstances around such re-admission.  Used in HL7 Version 2.x messagine in the PV1 segment.</t>
         </is>
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>ValueSet/v2-0116</t>
+          <t>ValueSet/v2-0092</t>
         </is>
       </c>
       <c r="I97" t="inlineStr"/>
@@ -4695,7 +4695,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v2-0131</t>
+          <t>http://terminology.hl7.org/CodeSystem/v2-0116</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -4710,27 +4710,27 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.18.58</t>
+          <t>2.16.840.1.113883.18.47</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>ContactRole2</t>
+          <t>BedStatus</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>contactRole2</t>
+          <t>bedStatus</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>Code system of concepts which specify a relationship role that the next of kin/associated parties plays with regard to the patient. Also used in referrals, for example, it may be necessary to identify the contact representative at the clinic that sent a referral. Used in HL7 Version 2 messaging in the NK1 and CTD segments after 2.5, when it replace 2.16.840.1.113883.18.57.</t>
+          <t>Code system of concepts which specify the state of a bed in an inpatient setting, and is used to determine if a patient may be assigned to it or not.  Used in HL7 Version 2.x messaging in the DLD and PV1 segments.</t>
         </is>
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>ValueSet/relatedperson-relationshiptype,ValueSet/patient-contactrelationship</t>
+          <t>ValueSet/v2-0116</t>
         </is>
       </c>
       <c r="I98" t="inlineStr"/>
@@ -4739,12 +4739,12 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v2-0203</t>
+          <t>http://terminology.hl7.org/CodeSystem/v2-0131</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>4.0.0</t>
+          <t>2.0.0</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -4754,27 +4754,27 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.18.108</t>
+          <t>2.16.840.1.113883.18.58</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>IdentifierType</t>
+          <t>ContactRole2</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>identifierType</t>
+          <t>contactRole2</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>HL7-defined code system of concepts specifying type of identifier. Used in HL7 Version 2.x messaging data types CX, PLN, PPN, XCN and XON.</t>
+          <t>Code system of concepts which specify a relationship role that the next of kin/associated parties plays with regard to the patient. Also used in referrals, for example, it may be necessary to identify the contact representative at the clinic that sent a referral. Used in HL7 Version 2 messaging in the NK1 and CTD segments after 2.5, when it replace 2.16.840.1.113883.18.57.</t>
         </is>
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>ValueSet/identifier-type</t>
+          <t>ValueSet/relatedperson-relationshiptype,ValueSet/patient-contactrelationship</t>
         </is>
       </c>
       <c r="I99" t="inlineStr"/>
@@ -4783,12 +4783,12 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v2-0371</t>
+          <t>http://terminology.hl7.org/CodeSystem/v2-0203</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>2.0.0</t>
+          <t>4.0.0</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -4798,27 +4798,27 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.18.229</t>
+          <t>2.16.840.1.113883.18.108</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>AdditivePreservative</t>
+          <t>IdentifierType</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>additivePreservative</t>
+          <t>identifierType</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>HL7-defined code system of concepts specifying any additive introduced to the specimen before or at the time of collection.  These additives may be introduced in order to preserve, maintain or enhance the particular nature or component of the specimen.  Used in HL7 Version 2.x messaging in the SPM and SAC segments.</t>
+          <t>HL7-defined code system of concepts specifying type of identifier. Used in HL7 Version 2.x messaging data types CX, PLN, PPN, XCN and XON.</t>
         </is>
       </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t>ValueSet/v2-0371</t>
+          <t>ValueSet/identifier-type</t>
         </is>
       </c>
       <c r="I100" t="inlineStr"/>
@@ -4827,7 +4827,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v2-0373</t>
+          <t>http://terminology.hl7.org/CodeSystem/v2-0371</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -4842,27 +4842,27 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.18.231</t>
+          <t>2.16.840.1.113883.18.229</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Treatment</t>
+          <t>AdditivePreservative</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>treatment</t>
+          <t>additivePreservative</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>Code system of concepts that identify the specimen treatment performed during lab processing.  Used in the Interaction Specimen Container Detail (SAC) segment in HL7 Version 2.x messaging.</t>
+          <t>HL7-defined code system of concepts specifying any additive introduced to the specimen before or at the time of collection.  These additives may be introduced in order to preserve, maintain or enhance the particular nature or component of the specimen.  Used in HL7 Version 2.x messaging in the SPM and SAC segments.</t>
         </is>
       </c>
       <c r="H101" t="inlineStr">
         <is>
-          <t>ValueSet/specimen-processing-procedure</t>
+          <t>ValueSet/v2-0371</t>
         </is>
       </c>
       <c r="I101" t="inlineStr"/>
@@ -4871,7 +4871,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v2-0443</t>
+          <t>http://terminology.hl7.org/CodeSystem/v2-0373</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -4886,27 +4886,27 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.18.283</t>
+          <t>2.16.840.1.113883.18.231</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>ProviderRole</t>
+          <t>Treatment</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>providerRole</t>
+          <t>treatment</t>
         </is>
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>Code system of concepts specifying the functional involvement with the activity being transmitted (e.g., Case Manager, Evaluator, Transcriber, Nurse Care Practitioner, Midwife, Physician Assistant, etc.).  Used in HL7 Version 2.x messaging in the ROL segment.</t>
+          <t>Code system of concepts that identify the specimen treatment performed during lab processing.  Used in the Interaction Specimen Container Detail (SAC) segment in HL7 Version 2.x messaging.</t>
         </is>
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>ValueSet/immunization-function</t>
+          <t>ValueSet/specimen-processing-procedure</t>
         </is>
       </c>
       <c r="I102" t="inlineStr"/>
@@ -4915,7 +4915,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v2-0916</t>
+          <t>http://terminology.hl7.org/CodeSystem/v2-0443</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -4930,27 +4930,27 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.18.422</t>
+          <t>2.16.840.1.113883.18.283</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>RelevantClincialInformation</t>
+          <t>ProviderRole</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>relevantClincialInformation</t>
+          <t>providerRole</t>
         </is>
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>Code system of concepts specifying additional clinical information about the patient or specimen to report the supporting and/or suspected diagnosis and clinical findings on requests for interpreted diagnostic studies. Used in HL7 Version 2.x messaging in the OBR segment.</t>
+          <t>Code system of concepts specifying the functional involvement with the activity being transmitted (e.g., Case Manager, Evaluator, Transcriber, Nurse Care Practitioner, Midwife, Physician Assistant, etc.).  Used in HL7 Version 2.x messaging in the ROL segment.</t>
         </is>
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>ValueSet/v2-0916</t>
+          <t>ValueSet/immunization-function</t>
         </is>
       </c>
       <c r="I103" t="inlineStr"/>
@@ -4959,12 +4959,12 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v3-ActCode</t>
+          <t>http://terminology.hl7.org/CodeSystem/v2-0916</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>9.0.0</t>
+          <t>2.0.0</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -4974,27 +4974,27 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.5.4</t>
+          <t>2.16.840.1.113883.18.422</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>ActCode</t>
+          <t>RelevantClincialInformation</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>ActCode</t>
+          <t>relevantClincialInformation</t>
         </is>
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>A code specifying the particular kind of Act that the Act-instance represents within its class.    *Constraints:* The kind of Act (e.g. physical examination, serum potassium, inpatient encounter, charge financial transaction, etc.) is specified with a code from one of several, typically external, coding systems. The coding system will depend on the class of Act, such as LOINC for observations, etc.    Conceptually, the Act.code must be a specialization of the Act.classCode. This is why the structure of ActClass domain should be reflected in the superstructure of the ActCode domain and then individual codes or externally referenced vocabularies subordinated under these domains that reflect the ActClass structure.    Act.classCode and Act.code are not modifiers of each other but the Act.code concept should really imply the Act.classCode concept. For a negative example, it is not appropriate to use an Act.code "potassium" together with and Act.classCode for "laboratory observation" to somehow mean "potassium laboratory observation" and then use the same Act.code for "potassium" together with Act.classCode for "medication" to mean "substitution of potassium". This mutually modifying use of Act.code and Act.classCode is not permitted.</t>
+          <t>Code system of concepts specifying additional clinical information about the patient or specimen to report the supporting and/or suspected diagnosis and clinical findings on requests for interpreted diagnostic studies. Used in HL7 Version 2.x messaging in the OBR segment.</t>
         </is>
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>ValueSet/v3-ActPharmacySupplyType,ValueSet/v3-ActCode,ValueSet/provenance-activity-type,ValueSet/v3-ActEncounterCode</t>
+          <t>ValueSet/v2-0916</t>
         </is>
       </c>
       <c r="I104" t="inlineStr"/>
@@ -5003,12 +5003,12 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v3-ActPriority</t>
+          <t>http://terminology.hl7.org/CodeSystem/v3-ActCode</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>3.0.0</t>
+          <t>9.0.0</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -5018,27 +5018,27 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.5.7</t>
+          <t>2.16.840.1.113883.5.4</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>ActPriority</t>
+          <t>ActCode</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>ActPriority</t>
+          <t>ActCode</t>
         </is>
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>A set of codes (e.g., for routine, emergency), specifying the urgency under which the Act happened, can happen, is happening, is intended to happen, or is requested/demanded to happen.</t>
+          <t>A code specifying the particular kind of Act that the Act-instance represents within its class.    *Constraints:* The kind of Act (e.g. physical examination, serum potassium, inpatient encounter, charge financial transaction, etc.) is specified with a code from one of several, typically external, coding systems. The coding system will depend on the class of Act, such as LOINC for observations, etc.    Conceptually, the Act.code must be a specialization of the Act.classCode. This is why the structure of ActClass domain should be reflected in the superstructure of the ActCode domain and then individual codes or externally referenced vocabularies subordinated under these domains that reflect the ActClass structure.    Act.classCode and Act.code are not modifiers of each other but the Act.code concept should really imply the Act.classCode concept. For a negative example, it is not appropriate to use an Act.code "potassium" together with and Act.classCode for "laboratory observation" to somehow mean "potassium laboratory observation" and then use the same Act.code for "potassium" together with Act.classCode for "medication" to mean "substitution of potassium". This mutually modifying use of Act.code and Act.classCode is not permitted.</t>
         </is>
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>ValueSet/v3-ActPriority</t>
+          <t>ValueSet/v3-ActPharmacySupplyType,ValueSet/v3-ActCode,ValueSet/provenance-activity-type,ValueSet/v3-ActEncounterCode</t>
         </is>
       </c>
       <c r="I105" t="inlineStr"/>
@@ -5047,12 +5047,12 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v3-ActReason</t>
+          <t>http://terminology.hl7.org/CodeSystem/v3-ActPriority</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>3.1.0</t>
+          <t>3.0.0</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -5062,27 +5062,27 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.5.8</t>
+          <t>2.16.840.1.113883.5.7</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>ActReason</t>
+          <t>ActPriority</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>ActReason</t>
+          <t>ActPriority</t>
         </is>
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>A set of codes specifying the motivation, cause, or rationale of an Act, when such rationale is not reasonably represented as an ActRelationship of type "has reason" linking to another Act.    *Examples:* Example reasons that might qualify for being coded in this field might be: "routine requirement", "infectious disease reporting requirement", "on patient request", "required by law".</t>
+          <t>A set of codes (e.g., for routine, emergency), specifying the urgency under which the Act happened, can happen, is happening, is intended to happen, or is requested/demanded to happen.</t>
         </is>
       </c>
       <c r="H106" t="inlineStr">
         <is>
-          <t>ValueSet/immunization-status-reason,ValueSet/v3-PurposeOfUse,ValueSet/v3-SubstanceAdminSubstitutionReason</t>
+          <t>ValueSet/v3-ActPriority</t>
         </is>
       </c>
       <c r="I106" t="inlineStr"/>
@@ -5091,12 +5091,12 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v3-ActSite</t>
+          <t>http://terminology.hl7.org/CodeSystem/v3-ActReason</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>3.0.0</t>
+          <t>3.1.0</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -5106,27 +5106,27 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.5.1052</t>
+          <t>2.16.840.1.113883.5.8</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>ActSite</t>
+          <t>ActReason</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>ActSite</t>
+          <t>ActReason</t>
         </is>
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>An anatomical location on an organism which can be the focus of an act.</t>
+          <t>A set of codes specifying the motivation, cause, or rationale of an Act, when such rationale is not reasonably represented as an ActRelationship of type "has reason" linking to another Act.    *Examples:* Example reasons that might qualify for being coded in this field might be: "routine requirement", "infectious disease reporting requirement", "on patient request", "required by law".</t>
         </is>
       </c>
       <c r="H107" t="inlineStr">
         <is>
-          <t>ValueSet/immunization-site</t>
+          <t>ValueSet/v3-PurposeOfUse,ValueSet/immunization-status-reason,ValueSet/v3-SubstanceAdminSubstitutionReason</t>
         </is>
       </c>
       <c r="I107" t="inlineStr"/>
@@ -5135,12 +5135,12 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v3-DataOperation</t>
+          <t>http://terminology.hl7.org/CodeSystem/v3-ActSite</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>5.0.0</t>
+          <t>3.0.0</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -5150,27 +5150,27 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.5.1123</t>
+          <t>2.16.840.1.113883.5.1052</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>DataOperation</t>
+          <t>ActSite</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>DataOperation</t>
+          <t>ActSite</t>
         </is>
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>**** MISSING DESCRIPTION ****</t>
+          <t>An anatomical location on an organism which can be the focus of an act.</t>
         </is>
       </c>
       <c r="H108" t="inlineStr">
         <is>
-          <t>ValueSet/provenance-activity-type</t>
+          <t>ValueSet/immunization-site</t>
         </is>
       </c>
       <c r="I108" t="inlineStr"/>
@@ -5179,12 +5179,12 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v3-DocumentCompletion</t>
+          <t>http://terminology.hl7.org/CodeSystem/v3-DataOperation</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>3.0.0</t>
+          <t>5.0.0</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -5194,22 +5194,22 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.5.33</t>
+          <t>2.16.840.1.113883.5.1123</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>DocumentCompletion</t>
+          <t>DataOperation</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>DocumentCompletion</t>
+          <t>DataOperation</t>
         </is>
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>Identifies the current completion state of a clinical document.</t>
+          <t>**** MISSING DESCRIPTION ****</t>
         </is>
       </c>
       <c r="H109" t="inlineStr">
@@ -5223,7 +5223,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v3-EncounterSpecialCourtesy</t>
+          <t>http://terminology.hl7.org/CodeSystem/v3-DocumentCompletion</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -5238,27 +5238,27 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.5.40</t>
+          <t>2.16.840.1.113883.5.33</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>EncounterSpecialCourtesy</t>
+          <t>DocumentCompletion</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>EncounterSpecialCourtesy</t>
+          <t>DocumentCompletion</t>
         </is>
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>**** MISSING DESCRIPTION ****</t>
+          <t>Identifies the current completion state of a clinical document.</t>
         </is>
       </c>
       <c r="H110" t="inlineStr">
         <is>
-          <t>ValueSet/encounter-special-courtesy</t>
+          <t>ValueSet/provenance-activity-type</t>
         </is>
       </c>
       <c r="I110" t="inlineStr"/>
@@ -5267,12 +5267,12 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v3-HL7DocumentFormatCodes</t>
+          <t>http://terminology.hl7.org/CodeSystem/v3-EncounterSpecialCourtesy</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>4.0.0</t>
+          <t>3.0.0</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -5282,27 +5282,27 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.1.1407</t>
+          <t>2.16.840.1.113883.5.40</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>HL7DocumentFormatCodes</t>
+          <t>EncounterSpecialCourtesy</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>HL7 Document Format Codes</t>
+          <t>EncounterSpecialCourtesy</t>
         </is>
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>This codeSystem contains codes which specify the technical format of a document. Each code provides sufficient information to allow any potential document consumer to know if it will be able to process the document. The codes are sufficiently specific to ensure processing/display by identifying a document encoding, structure and template. For example, formatCodes can be used in the FHIR DocumentReference resource to characterize the document being referenced.</t>
+          <t>**** MISSING DESCRIPTION ****</t>
         </is>
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>ValueSet/v3-HL7FormatCodes</t>
+          <t>ValueSet/encounter-special-courtesy</t>
         </is>
       </c>
       <c r="I111" t="inlineStr"/>
@@ -5311,12 +5311,12 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v3-MaritalStatus</t>
+          <t>http://terminology.hl7.org/CodeSystem/v3-HL7DocumentFormatCodes</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>3.0.0</t>
+          <t>4.1.0</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -5326,27 +5326,27 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.5.2</t>
+          <t>2.16.840.1.113883.4.642.1.1407</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>MaritalStatus</t>
+          <t>HL7DocumentFormatCodes</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>MaritalStatus</t>
+          <t>HL7 Document Format Codes</t>
         </is>
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>\* \* \* No description supplied \* \* \*    *Open Issue:* The specific meanings of these codes can vary somewhat by jurisdiction and implementation so caution should be used when determining equivalency.    *Open Issue:* fixing and completion of the hierarchy and proper good definitions of all the concepts is badly needed.</t>
+          <t>This codeSystem contains codes which specify the technical format of a document. Each code provides sufficient information to allow any potential document consumer to know if it will be able to process the document. The codes are sufficiently specific to ensure processing/display by identifying a document encoding, structure and template. For example, formatCodes can be used in the FHIR DocumentReference resource to characterize the document being referenced.</t>
         </is>
       </c>
       <c r="H112" t="inlineStr">
         <is>
-          <t>ValueSet/marital-status</t>
+          <t>ValueSet/v3-HL7FormatCodes</t>
         </is>
       </c>
       <c r="I112" t="inlineStr"/>
@@ -5355,7 +5355,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v3-NullFlavor</t>
+          <t>http://terminology.hl7.org/CodeSystem/v3-MaritalStatus</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -5370,27 +5370,27 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.5.1008</t>
+          <t>2.16.840.1.113883.5.2</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>NullFlavor</t>
+          <t>MaritalStatus</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>NullFlavor</t>
+          <t>MaritalStatus</t>
         </is>
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>A collection of codes specifying why a valid value is not present.</t>
+          <t>\* \* \* No description supplied \* \* \*    *Open Issue:* The specific meanings of these codes can vary somewhat by jurisdiction and implementation so caution should be used when determining equivalency.    *Open Issue:* fixing and completion of the hierarchy and proper good definitions of all the concepts is badly needed.</t>
         </is>
       </c>
       <c r="H113" t="inlineStr">
         <is>
-          <t>ValueSet/us-core-documentreference-type,ValueSet/marital-status,ValueSet/encounter-special-courtesy</t>
+          <t>ValueSet/marital-status</t>
         </is>
       </c>
       <c r="I113" t="inlineStr"/>
@@ -5399,7 +5399,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v3-ObservationInterpretation</t>
+          <t>http://terminology.hl7.org/CodeSystem/v3-NullFlavor</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -5414,27 +5414,27 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.5.83</t>
+          <t>2.16.840.1.113883.5.1008</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>ObservationInterpretation</t>
+          <t>NullFlavor</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>ObservationInterpretation</t>
+          <t>NullFlavor</t>
         </is>
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>One or more codes providing a rough qualitative interpretation of the observation, such as "normal" / "abnormal", "low" / "high", "better" / "worse", "resistant" / "susceptible", "expected" / "not expected". The value set is intended to be for ANY use where coded representation of an interpretation is needed.</t>
+          <t>A collection of codes specifying why a valid value is not present.</t>
         </is>
       </c>
       <c r="H114" t="inlineStr">
         <is>
-          <t>ValueSet/observation-interpretation</t>
+          <t>ValueSet/us-core-documentreference-type,ValueSet/marital-status,ValueSet/encounter-special-courtesy</t>
         </is>
       </c>
       <c r="I114" t="inlineStr"/>
@@ -5443,7 +5443,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v3-ParticipationFunction</t>
+          <t>http://terminology.hl7.org/CodeSystem/v3-ObservationInterpretation</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -5458,27 +5458,27 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.5.88</t>
+          <t>2.16.840.1.113883.5.83</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>ParticipationFunction</t>
+          <t>ObservationInterpretation</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>ParticipationFunction</t>
+          <t>ObservationInterpretation</t>
         </is>
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>This code is used to specify the exact function an actor had in a service in all necessary detail. This domain may include local extensions (CWE).</t>
+          <t>One or more codes providing a rough qualitative interpretation of the observation, such as "normal" / "abnormal", "low" / "high", "better" / "worse", "resistant" / "susceptible", "expected" / "not expected". The value set is intended to be for ANY use where coded representation of an interpretation is needed.</t>
         </is>
       </c>
       <c r="H115" t="inlineStr">
         <is>
-          <t>ValueSet/security-role-type</t>
+          <t>ValueSet/observation-interpretation</t>
         </is>
       </c>
       <c r="I115" t="inlineStr"/>
@@ -5487,12 +5487,12 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v3-ParticipationType</t>
+          <t>http://terminology.hl7.org/CodeSystem/v3-ParticipationFunction</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>5.0.0</t>
+          <t>3.0.0</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -5502,27 +5502,27 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.5.90</t>
+          <t>2.16.840.1.113883.5.88</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>ParticipationType</t>
+          <t>ParticipationFunction</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>ParticipationType</t>
+          <t>ParticipationFunction</t>
         </is>
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>A code specifying the meaning and purpose of every Participation instance. Each of its values implies specific constraints on the Roles undertaking the participation.</t>
+          <t>This code is used to specify the exact function an actor had in a service in all necessary detail. This domain may include local extensions (CWE).</t>
         </is>
       </c>
       <c r="H116" t="inlineStr">
         <is>
-          <t>ValueSet/security-role-type,ValueSet/encounter-participant-type,ValueSet/provenance-activity-type</t>
+          <t>ValueSet/security-role-type</t>
         </is>
       </c>
       <c r="I116" t="inlineStr"/>
@@ -5531,12 +5531,12 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v3-RoleClass</t>
+          <t>http://terminology.hl7.org/CodeSystem/v3-ParticipationType</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>4.0.0</t>
+          <t>5.0.0</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -5546,27 +5546,27 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.5.110</t>
+          <t>2.16.840.1.113883.5.90</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>RoleClass</t>
+          <t>ParticipationType</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>RoleClass</t>
+          <t>ParticipationType</t>
         </is>
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>Codes for the Role class hierarchy. The values in this hierarchy, represent a Role which is an association or relationship between two entities - the entity that plays the role and the entity that scopes the role. Roles names are derived from the name of the playing entity in that role.    The role hierarchy stems from three core concepts, or abstract domains:     *  **RoleClassOntological** is an abstract domain that collects roles in which the playing entity is defined or specified by the scoping entity.   *  **RoleClassPartitive** collects roles in which the playing entity is in some sense a "part" of the scoping entity.   *  **RoleClassAssociative** collects all of the remaining forms of association between the playing entity and the scoping entity. This set of roles is further partitioned between:             *  **RoleClassPassive** which are roles in which the playing entity is used, known, treated, handled, built, or destroyed, etc. under the auspices of the scoping entity. The playing entity is passive in these roles in that the role exists without an agreement from the playing entity.       *  **RoleClassMutualRelationship** which are relationships based on mutual behavior of the two entities. The basis of these relationship may be formal agreements or they may be *de facto* behavior. Thus, this sub-domain is further divided into:                     *  **RoleClassRelationshipFormal** in which the relationship is formally defined, frequently by a contract or agreement.           *  **Personal relationship** which inks two people in a personal relationship.    The hierarchy discussed above is represented In the current vocabulary tables as a set of abstract domains, with the exception of the "Personal relationship" which is a leaf concept.    *OpenIssue:* Description copied from Concept Domain of same name. Must be verified.</t>
+          <t>A code specifying the meaning and purpose of every Participation instance. Each of its values implies specific constraints on the Roles undertaking the participation.</t>
         </is>
       </c>
       <c r="H117" t="inlineStr">
         <is>
-          <t>ValueSet/security-role-type</t>
+          <t>ValueSet/security-role-type,ValueSet/encounter-participant-type,ValueSet/provenance-activity-type</t>
         </is>
       </c>
       <c r="I117" t="inlineStr"/>
@@ -5575,12 +5575,12 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v3-RoleCode</t>
+          <t>http://terminology.hl7.org/CodeSystem/v3-RoleClass</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>3.0.0</t>
+          <t>4.0.0</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -5590,27 +5590,27 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.5.111</t>
+          <t>2.16.840.1.113883.5.110</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>RoleCode</t>
+          <t>RoleClass</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>RoleCode</t>
+          <t>RoleClass</t>
         </is>
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>A set of codes further specifying the kind of Role; specific classification codes for further qualifying RoleClass codes.</t>
+          <t>Codes for the Role class hierarchy. The values in this hierarchy, represent a Role which is an association or relationship between two entities - the entity that plays the role and the entity that scopes the role. Roles names are derived from the name of the playing entity in that role.    The role hierarchy stems from three core concepts, or abstract domains:     *  **RoleClassOntological** is an abstract domain that collects roles in which the playing entity is defined or specified by the scoping entity.   *  **RoleClassPartitive** collects roles in which the playing entity is in some sense a "part" of the scoping entity.   *  **RoleClassAssociative** collects all of the remaining forms of association between the playing entity and the scoping entity. This set of roles is further partitioned between:             *  **RoleClassPassive** which are roles in which the playing entity is used, known, treated, handled, built, or destroyed, etc. under the auspices of the scoping entity. The playing entity is passive in these roles in that the role exists without an agreement from the playing entity.       *  **RoleClassMutualRelationship** which are relationships based on mutual behavior of the two entities. The basis of these relationship may be formal agreements or they may be *de facto* behavior. Thus, this sub-domain is further divided into:                     *  **RoleClassRelationshipFormal** in which the relationship is formally defined, frequently by a contract or agreement.           *  **Personal relationship** which inks two people in a personal relationship.    The hierarchy discussed above is represented In the current vocabulary tables as a set of abstract domains, with the exception of the "Personal relationship" which is a leaf concept.    *OpenIssue:* Description copied from Concept Domain of same name. Must be verified.</t>
         </is>
       </c>
       <c r="H118" t="inlineStr">
         <is>
-          <t>ValueSet/security-role-type,ValueSet/relatedperson-relationshiptype,ValueSet/v3-ServiceDeliveryLocationRoleType</t>
+          <t>ValueSet/security-role-type</t>
         </is>
       </c>
       <c r="I118" t="inlineStr"/>
@@ -5619,7 +5619,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v3-RouteOfAdministration</t>
+          <t>http://terminology.hl7.org/CodeSystem/v3-RoleCode</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -5634,27 +5634,27 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.5.112</t>
+          <t>2.16.840.1.113883.5.111</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>RouteOfAdministration</t>
+          <t>RoleCode</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>RouteOfAdministration</t>
+          <t>RoleCode</t>
         </is>
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>The path the administered medication takes to get into the body or into contact with the body.</t>
+          <t>A set of codes further specifying the kind of Role; specific classification codes for further qualifying RoleClass codes.</t>
         </is>
       </c>
       <c r="H119" t="inlineStr">
         <is>
-          <t>ValueSet/immunization-route</t>
+          <t>ValueSet/security-role-type,ValueSet/relatedperson-relationshiptype,ValueSet/v3-ServiceDeliveryLocationRoleType</t>
         </is>
       </c>
       <c r="I119" t="inlineStr"/>
@@ -5663,12 +5663,12 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v3-TribalEntityUS</t>
+          <t>http://terminology.hl7.org/CodeSystem/v3-RouteOfAdministration</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>4.0.0</t>
+          <t>3.0.0</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -5678,27 +5678,27 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.5.140</t>
+          <t>2.16.840.1.113883.5.112</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>TribalEntityUS</t>
+          <t>RouteOfAdministration</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>TribalEntityUS</t>
+          <t>RouteOfAdministration</t>
         </is>
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>INDIAN ENTITIES RECOGNIZED AND ELIGIBLE TO RECEIVE SERVICES FROM THE UNITED STATES BUREAU OF INDIAN AFFAIRS</t>
+          <t>The path the administered medication takes to get into the body or into contact with the body.</t>
         </is>
       </c>
       <c r="H120" t="inlineStr">
         <is>
-          <t>ValueSet/v3-TribalEntityUS</t>
+          <t>ValueSet/immunization-route</t>
         </is>
       </c>
       <c r="I120" t="inlineStr"/>
@@ -5707,12 +5707,12 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/CodeSystem/v3-substanceAdminSubstitution</t>
+          <t>http://terminology.hl7.org/CodeSystem/v3-TribalEntityUS</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>3.0.0</t>
+          <t>4.0.0</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -5722,27 +5722,27 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.5.1070</t>
+          <t>2.16.840.1.113883.5.140</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>SubstanceAdminSubstitution</t>
+          <t>TribalEntityUS</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>Substance Admin Substitution</t>
+          <t>TribalEntityUS</t>
         </is>
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>Identifies what sort of change is permitted or has occurred between the therapy that was ordered and the therapy that was/will be provided.</t>
+          <t>INDIAN ENTITIES RECOGNIZED AND ELIGIBLE TO RECEIVE SERVICES FROM THE UNITED STATES BUREAU OF INDIAN AFFAIRS</t>
         </is>
       </c>
       <c r="H121" t="inlineStr">
         <is>
-          <t>ValueSet/v3-ActSubstanceAdminSubstitutionCode</t>
+          <t>ValueSet/v3-TribalEntityUS</t>
         </is>
       </c>
       <c r="I121" t="inlineStr"/>
@@ -5751,42 +5751,42 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/fhir/CodeSystem/medicationdispense-category</t>
+          <t>http://terminology.hl7.org/CodeSystem/v3-substanceAdminSubstitution</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>4.0.1</t>
+          <t>3.0.0</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>draft</t>
+          <t>active</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.4.1315</t>
+          <t>2.16.840.1.113883.5.1070</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>MedicationDispense Category Codes</t>
+          <t>SubstanceAdminSubstitution</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>Medication dispense  category  codes</t>
+          <t>Substance Admin Substitution</t>
         </is>
       </c>
       <c r="G122" t="inlineStr">
         <is>
-          <t>MedicationDispense Category Codes</t>
+          <t>Identifies what sort of change is permitted or has occurred between the therapy that was ordered and the therapy that was/will be provided.</t>
         </is>
       </c>
       <c r="H122" t="inlineStr">
         <is>
-          <t>ValueSet/medicationdispense-category</t>
+          <t>ValueSet/v3-ActSubstanceAdminSubstitutionCode</t>
         </is>
       </c>
       <c r="I122" t="inlineStr"/>
@@ -5795,7 +5795,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/fhir/CodeSystem/medicationdispense-status-reason</t>
+          <t>http://terminology.hl7.org/fhir/CodeSystem/medicationdispense-category</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -5810,27 +5810,27 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.4.642.4.1317</t>
+          <t>2.16.840.1.113883.4.642.4.1315</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>MedicationDispense Status Reason Codes</t>
+          <t>MedicationDispense Category Codes</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>Medication dispense  status  reason  codes</t>
+          <t>Medication dispense  category  codes</t>
         </is>
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>MedicationDispense Status Codes</t>
+          <t>MedicationDispense Category Codes</t>
         </is>
       </c>
       <c r="H123" t="inlineStr">
         <is>
-          <t>ValueSet/medicationdispense-status-reason</t>
+          <t>ValueSet/medicationdispense-category</t>
         </is>
       </c>
       <c r="I123" t="inlineStr"/>
@@ -5839,42 +5839,42 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>http://unitsofmeasure.org</t>
+          <t>http://terminology.hl7.org/fhir/CodeSystem/medicationdispense-status-reason</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>3.0.1</t>
+          <t>4.0.1</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>draft</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.6.8</t>
+          <t>2.16.840.1.113883.4.642.4.1317</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>UCUM</t>
+          <t>MedicationDispense Status Reason Codes</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>Unified Code for Units of Measure (UCUM)</t>
+          <t>Medication dispense  status  reason  codes</t>
         </is>
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>The Unified Code for Units of Measure (UCUM) is a code system intended to include all units of measures being contemporarily used in international science, engineering, and business. The purpose is to facilitate unambiguous electronic communication of quantities together with their units. The focus is on electronic communication, as opposed to communication between humans. A typical application of The Unified Code for Units of Measure are electronic data interchange (EDI) protocols, but there is nothing that prevents it from being used in other types of machine communication.</t>
+          <t>MedicationDispense Status Codes</t>
         </is>
       </c>
       <c r="H124" t="inlineStr">
         <is>
-          <t>ValueSet/ucum-bodyweight,ValueSet/ucum-bodytemp,ValueSet/ucum-common,ValueSet/ucum-vitals-common,ValueSet/v3-UnitsOfMeasureCaseSensitive,ValueSet/ucum-bodylength</t>
+          <t>ValueSet/medicationdispense-status-reason</t>
         </is>
       </c>
       <c r="I124" t="inlineStr"/>
@@ -5883,7 +5883,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>http://www.ada.org/cdt</t>
+          <t>http://unitsofmeasure.org</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -5898,27 +5898,27 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.6.13</t>
+          <t>2.16.840.1.113883.6.8</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>CDT</t>
+          <t>UCUM</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>Code on Dental Procedures and Nomenclature</t>
+          <t>Unified Code for Units of Measure (UCUM)</t>
         </is>
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>The purpose of the CDT Code is to achieve uniformity, consistency and specificity in accurately documenting dental treatment. One use of the CDT Code is to provide for the efficient processing of dental claims, and another is to populate an Electronic Health Record.</t>
+          <t>The Unified Code for Units of Measure (UCUM) is a code system intended to include all units of measures being contemporarily used in international science, engineering, and business. The purpose is to facilitate unambiguous electronic communication of quantities together with their units. The focus is on electronic communication, as opposed to communication between humans. A typical application of The Unified Code for Units of Measure are electronic data interchange (EDI) protocols, but there is nothing that prevents it from being used in other types of machine communication.</t>
         </is>
       </c>
       <c r="H125" t="inlineStr">
         <is>
-          <t>ValueSet/us-core-procedure-code</t>
+          <t>ValueSet/ucum-bodyweight,ValueSet/ucum-bodytemp,ValueSet/ucum-common,ValueSet/ucum-vitals-common,ValueSet/v3-UnitsOfMeasureCaseSensitive,ValueSet/ucum-bodylength</t>
         </is>
       </c>
       <c r="I125" t="inlineStr"/>
@@ -5927,7 +5927,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>http://www.ama-assn.org/go/cpt</t>
+          <t>http://www.ada.org/cdt</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -5942,22 +5942,22 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.6.12</t>
+          <t>2.16.840.1.113883.6.13</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>CPT</t>
+          <t>CDT</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>Current Procedural Terminology (CPT®)</t>
+          <t>Code on Dental Procedures and Nomenclature</t>
         </is>
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>The Current Procedural Terminology (CPT) code set, created and maintained by the American Medical Association, is the language of medicine today and the code to its future. This system of terminology is the most widely accepted medical nomenclature used to report medical procedures and services under public and private health insurance programs. CPT coding is also used for administrative management purposes such as claims processing and developing guidelines for medical care review. Each year, via a rigorous, evidence-based and transparent process, the independent CPT Editorial Panel revises, creates or deletes hundreds of codes in order to reflect current medical practice.    Designated by the U.S. Department of Health and Human Services under the Health Insurance Portability and Accountability Act (HIPAA) as a national coding set for physician and other health care professional services and procedures, CPT’s evidence-based codes accurately encompass the full range of health care services.    All CPT codes are five-digits and can be either numeric or alphanumeric, depending on the category. CPT code descriptors are clinically focused and utilize common standards so that a diverse set of users can have common understanding across the clinical health care paradigm.    There are various types of CPT codes:    Category I: These codes have descriptors that correspond to a procedure or service. Codes range from 00100–99499 and are generally ordered into sub-categories based on procedure/service type and anatomy.    Category II: These alphanumeric tracking codes are supplemental codes used for performance measurement. Using them is optional and not required for correct coding.    Category III: These are temporary alphanumeric codes for new and developing technology, procedures and services. They were created for data collection, assessment and in some instances, payment of new services and procedures that currently don’t meet the criteria for a Category I code.    Proprietary Laboratory Analyses (PLA) codes: These codes describe proprietary clinical laboratory analyses and can be either provided by a single (“solesource”) laboratory or licensed or marketed to multiple providing laboratories that are cleared or approved by the Food and Drug Administration (FDA)). This category includes but is not limited to Advanced Diagnostic Laboratory Tests (ADLTs) and Clinical Diagnostic Laboratory Tests (CDLTs), as defined under the Protecting Access to Medicare Act of 2014 (PAMA).</t>
+          <t>The purpose of the CDT Code is to achieve uniformity, consistency and specificity in accurately documenting dental treatment. One use of the CDT Code is to provide for the efficient processing of dental claims, and another is to populate an Electronic Health Record.</t>
         </is>
       </c>
       <c r="H126" t="inlineStr">
@@ -5971,12 +5971,12 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>http://www.cms.gov/Medicare/Coding/ICD10</t>
+          <t>http://www.ama-assn.org/go/cpt</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>2.0.1</t>
+          <t>3.0.1</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -5986,22 +5986,22 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.6.4</t>
+          <t>2.16.840.1.113883.6.12</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>Icd10PCS</t>
+          <t>CPT</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>ICD-10 Procedure Codes</t>
+          <t>Current Procedural Terminology (CPT®)</t>
         </is>
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>ICD Procedure Coding System (ICD 10 PCS)</t>
+          <t>The Current Procedural Terminology (CPT) code set, created and maintained by the American Medical Association, is the language of medicine today and the code to its future. This system of terminology is the most widely accepted medical nomenclature used to report medical procedures and services under public and private health insurance programs. CPT coding is also used for administrative management purposes such as claims processing and developing guidelines for medical care review. Each year, via a rigorous, evidence-based and transparent process, the independent CPT Editorial Panel revises, creates or deletes hundreds of codes in order to reflect current medical practice.    Designated by the U.S. Department of Health and Human Services under the Health Insurance Portability and Accountability Act (HIPAA) as a national coding set for physician and other health care professional services and procedures, CPT’s evidence-based codes accurately encompass the full range of health care services.    All CPT codes are five-digits and can be either numeric or alphanumeric, depending on the category. CPT code descriptors are clinically focused and utilize common standards so that a diverse set of users can have common understanding across the clinical health care paradigm.    There are various types of CPT codes:    Category I: These codes have descriptors that correspond to a procedure or service. Codes range from 00100–99499 and are generally ordered into sub-categories based on procedure/service type and anatomy.    Category II: These alphanumeric tracking codes are supplemental codes used for performance measurement. Using them is optional and not required for correct coding.    Category III: These are temporary alphanumeric codes for new and developing technology, procedures and services. They were created for data collection, assessment and in some instances, payment of new services and procedures that currently don’t meet the criteria for a Category I code.    Proprietary Laboratory Analyses (PLA) codes: These codes describe proprietary clinical laboratory analyses and can be either provided by a single (“solesource”) laboratory or licensed or marketed to multiple providing laboratories that are cleared or approved by the Food and Drug Administration (FDA)). This category includes but is not limited to Advanced Diagnostic Laboratory Tests (ADLTs) and Clinical Diagnostic Laboratory Tests (CDLTs), as defined under the Protecting Access to Medicare Act of 2014 (PAMA).</t>
         </is>
       </c>
       <c r="H127" t="inlineStr">
@@ -6015,11 +6015,13 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>https://nahdo.org/sopt</t>
-        </is>
-      </c>
-      <c r="B128" t="n">
-        <v>9.199999999999999</v>
+          <t>http://www.cms.gov/Medicare/Coding/ICD10</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>2.0.1</t>
+        </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
@@ -6028,23 +6030,27 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.3.221.5</t>
+          <t>2.16.840.1.113883.6.4</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>SOP</t>
+          <t>Icd10PCS</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>Source of Payment Typology</t>
-        </is>
-      </c>
-      <c r="G128" t="inlineStr"/>
+          <t>ICD-10 Procedure Codes</t>
+        </is>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>ICD Procedure Coding System (ICD 10 PCS)</t>
+        </is>
+      </c>
       <c r="H128" t="inlineStr">
         <is>
-          <t>ValueSet/2.16.840.1.114222.4.11.3591</t>
+          <t>ValueSet/us-core-procedure-code</t>
         </is>
       </c>
       <c r="I128" t="inlineStr"/>
@@ -6053,13 +6059,11 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>urn:ietf:bcp:47</t>
-        </is>
-      </c>
-      <c r="B129" t="inlineStr">
-        <is>
-          <t>2.0.1</t>
-        </is>
+          <t>https://nahdo.org/sopt</t>
+        </is>
+      </c>
+      <c r="B129" t="n">
+        <v>9.199999999999999</v>
       </c>
       <c r="C129" t="inlineStr">
         <is>
@@ -6068,31 +6072,109 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.6.121</t>
+          <t>2.16.840.1.113883.3.221.5</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>Ietf3066</t>
+          <t>SOP</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>Tags for the Identification of Languages</t>
-        </is>
-      </c>
-      <c r="G129" t="inlineStr">
-        <is>
-          <t>Older value from OID registry.  Superceded; see recommendations in BCP-47.</t>
-        </is>
-      </c>
+          <t>Source of Payment Typology</t>
+        </is>
+      </c>
+      <c r="G129" t="inlineStr"/>
       <c r="H129" t="inlineStr">
         <is>
-          <t>ValueSet/languages,ValueSet/simple-language</t>
+          <t>ValueSet/2.16.840.1.114222.4.11.3591</t>
         </is>
       </c>
       <c r="I129" t="inlineStr"/>
       <c r="J129" t="inlineStr"/>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>https://www.cdc.gov/nhsn/cdaportal/terminology/codesystem/hsloc.html</t>
+        </is>
+      </c>
+      <c r="B130" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>2.16.840.1.113883.6.259</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>HSLOC</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>Healthcare Service Location</t>
+        </is>
+      </c>
+      <c r="G130" t="inlineStr"/>
+      <c r="H130" t="inlineStr">
+        <is>
+          <t>ValueSet/2.16.840.1.113883.1.11.20275</t>
+        </is>
+      </c>
+      <c r="I130" t="inlineStr"/>
+      <c r="J130" t="inlineStr"/>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>urn:ietf:bcp:47</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>2.0.1</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>2.16.840.1.113883.6.121</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>Ietf3066</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>Tags for the Identification of Languages</t>
+        </is>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>Older value from OID registry.  Superceded; see recommendations in BCP-47.</t>
+        </is>
+      </c>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>ValueSet/languages,ValueSet/Languages</t>
+        </is>
+      </c>
+      <c r="I131" t="inlineStr"/>
+      <c r="J131" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>